<commit_message>
Uploading re-knit, updates to data collection
added 6 additional products with links in the spreadsheet.
</commit_message>
<xml_diff>
--- a/data/Data Collection.xlsx
+++ b/data/Data Collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pconn\OneDrive\Desktop\Data Mining\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC9352C-5B07-4EBD-90D2-79577F6B2EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC62B5DB-6473-486F-A05F-BB3AA5397EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="1" xr2:uid="{EFA0F3B4-3249-4998-8A76-0DCAF9FCE7B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="1" xr2:uid="{EFA0F3B4-3249-4998-8A76-0DCAF9FCE7B8}"/>
   </bookViews>
   <sheets>
     <sheet name="productCollectionList" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="177">
   <si>
     <t>id</t>
   </si>
@@ -525,6 +525,78 @@
   </si>
   <si>
     <t>https://www.target.com/p/lg-65-34-class-4k-uhd-2160p-smart-oled-tv-oled65c3/-/A-88196023</t>
+  </si>
+  <si>
+    <t>Hogwarts Legacy (XBOX)</t>
+  </si>
+  <si>
+    <t>Jedi Survivor PS5</t>
+  </si>
+  <si>
+    <t>MarioKart8 Deluxe - Switch</t>
+  </si>
+  <si>
+    <t>Ninja Woodfire Pizza Oven</t>
+  </si>
+  <si>
+    <t>Igloo 24qt Cooler</t>
+  </si>
+  <si>
+    <t>Dyson Ball Animal 3 Extra Upright Vacuum Cleaner</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/hogwarts-legacy-xbox-series-x/-/A-86267032</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/star-wars-jedi-survivor-playstation-5/-/A-88183520</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/mario-kart-8-deluxe-nintendo-switch/-/A-52161278</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/ninja-woodfire-pizza-oven-8-in-1-outdoor-oven-5-pizza-settings-smoker-ninja-woodfire-technology-electric-oo101/-/A-89401843</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/igloo-imx-24qt-cooler-meteorite/-/A-87378961</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/dyson-ball-animal-3-extra-upright-vacuum/-/A-85269264</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Hogwarts-Legacy-Xbox-English-Version-Region/dp/B0B9YSJC5S/ref=sr_1_2?crid=1K69XYMHWNR56&amp;dib=eyJ2IjoiMSJ9.Kg0XV9Kot63z1u2KagkEvpCVUtkbGXvapqAJX7afkiu3BdvCRxuMMxHq3-R-Vq88oqItB-jjTuSzsA4OUT3gHqxnGxm_W3ax9Bt1-kNDhIIrfk2DMuaREs1iW3ZpC41UpXGGXpnKaQWx_QR6PweYu_E0fgQaz6JOeKQrHgmpoGnZNkaPqUf-EzAWuLvi4LuOAF_AT5tsuZUIeboaBcrdGFpzu4TWaNBwkw4WmSvH7Vo.uFmuTgI86APUwJ8qSsprJqvZ4Dnr_EwLXhTo2K61-P0&amp;dib_tag=se&amp;keywords=hogwarts+legacy+xbox&amp;qid=1710278855&amp;sprefix=hogwarts+legacy+xbox%2Caps%2C129&amp;sr=8-2</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Star-Wars-Jedi-Survivor-Playstation-5/dp/B0BPD4JMWT/ref=sr_1_1?crid=1YEWINBQP33M2&amp;dib=eyJ2IjoiMSJ9.xmgn1bEBQh8fF6vN-_ijDTx3NnKfAvuz4KzU8chGgsL67cKZ-GVbOSb0nGWeW8mxQpNntErtqMVDRP2_Qvv6NVonWyAdXrQOG1vF3pQuiK5vfmslLzeTXkEtyMSwY0hE5dvkCY4Udzheb9VLdQgjV4RNjelCbXWMWS3HDuqkxw8RhbOBcyBB1KuJpYwpU0LO3JbTFOrTQoCecarfSPAyc01kEOKHqvHzXAHZPHjTRpo.vqAgJHJ_EuyQ0aHKHSEiLA9mvUUFdQtDGBvQua34gew&amp;dib_tag=se&amp;keywords=jedi+survivor+ps5&amp;qid=1710278950&amp;sprefix=jedi+survivor+ps%2Caps%2C174&amp;sr=8-1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Mario-Kart-8-Deluxe-Nintendo-Switch/dp/B01N1037CV/ref=sr_1_1?crid=1PYFQU1N4B68F&amp;dib=eyJ2IjoiMSJ9.8TZU_Of0o7Vk3YWNjDE9oY9I_W3GMrGxHT454fa05jnyQhIJ1QoKGzaub95DXly85ZIxHf3U7vByBD9UHUHObxJwp-_uYmPTubto19uqmmQglLhYd3W-DOvMZz4lfv1l9ezRsNuuryHtJljvddmeIZdaJWrxpna-VU5FHp3braflTwk_ypjvU7neyKr_vIay2KHtiMOKVjqNxAnzmGjWABX-bq-mvp-ghJ0Hq7eY9h4.vohI6h3tcX_pnwUMLahacLD3yr74bAsNKv9eeH5rAp0&amp;dib_tag=se&amp;keywords=mario+kart+8+deluxe&amp;qid=1710279189&amp;sprefix=mario+kart+%2Caps%2C167&amp;sr=8-1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Ninja-Woodfire-Technology-terracotta-OO101/dp/B0C6BQVDX3/ref=sr_1_3?crid=3DXGBNWLVTJHJ&amp;dib=eyJ2IjoiMSJ9.0WxsIb1exp9JW6Y3VWlsjnd4AbzdLgvTZ3dzGlCYh7z1OEIvxums8Mey72f26ju-BWrkrofq9sMNvCk49njaQbu-SN8ItGFSBFcq-t91Hsb6AE3rPWtoewiMwvt1h2JtkHhsZTKkYeLo0Y9nnD_eJ4STJOza34YIVUe9YB7S8nTqDnhXuTlMQ4TE6pHn3CnUHoVNJGIlgiU2ncUCADPEKpW5C2f1-rC8jpiw7k3qXsE.uqci_nwiB33tgkfGHQRjqPWrYYjoEoVkB-fSO930oYQ&amp;dib_tag=se&amp;keywords=Ninja%2BWoodfire%2BPizza%2BOven%2C%2B8-in-1%2BOutdoor%2BOven&amp;qid=1710280162&amp;sprefix=ninja%2Bwoodfire%2Bpizza%2Boven%2C%2B8-in-1%2Boutdoor%2Boven%2Caps%2C183&amp;sr=8-3&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B08YS7QZLL/ref=twister_B09V6MDSN6?_encoding=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Dyson-Animal-Extra-Upright-Vacuum/dp/B0B57QV5TT/ref=sr_1_3?crid=2IQWXZR08I144&amp;dib=eyJ2IjoiMSJ9.t3iEOoxEJUwLPVoSUcRptqioH5l2EvX8s4APBjqpAjI4e18xB7pmNY8TyLEanhvfvEQqqscP3Xi13oKWZQuQ1MaGTAAh82rbXWBT5nZjBYQqPFp7PUAvYcMk9RslrAyAZS0Nwv3r6RQ8M2iBSK7DQAZmAK0ycSydB1nB1cVDRVBJ0bgIwOtJPiE6ohrQceFbK44RLbkqiNcgSv_YM7QC30n8grFBmSgixz1fAwZtEd8.ZIHRSLxkS_22b7rx1F4ymcSJXsCEuBy_aVi0A1DzCpU&amp;dib_tag=se&amp;keywords=Dyson%2B-%2BBall%2BAnimal%2B3%2BExtra%2BUpright&amp;qid=1710280601&amp;sprefix=dyson%2B-%2Bball%2Banimal%2B3%2Bextra%2Bupright%2Caps%2C176&amp;sr=8-3&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/hogwarts-legacy-standard-edition-xbox-series-x/6502627.p?skuId=6502627</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/star-wars-jedi-survivor-standard-edition-playstation-5/6528657.p?skuId=6528657</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/mario-kart-8-deluxe-nintendo-switch/5723304.p?skuId=5723304</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/igloo-imx-24-quart-cooler-gray/6523836.p?skuId=6523836</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/dyson-ball-animal-3-extra-upright-vacuum-with-5-accessories-copper-silver/6504485.p?skuId=6504485</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/ninja-woodfire-pizza-oven-8-in-1-outdoor-oven-5-pizza-settings-700f-smoker-woodfire-technology-electric-terracotta-red/6548901.p?skuId=6548901</t>
   </si>
 </sst>
 </file>
@@ -623,10 +695,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -948,9 +1016,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBB0BCB-A94A-4B82-A2E9-B3B98544ABD5}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:B15"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1142,7 +1210,9 @@
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
         <v>28</v>
@@ -1152,7 +1222,9 @@
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>29</v>
@@ -1162,7 +1234,9 @@
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
         <v>30</v>
@@ -1172,7 +1246,9 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>31</v>
@@ -1182,7 +1258,9 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
@@ -1190,7 +1268,9 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
@@ -1371,11 +1451,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8FFCC8-FB4D-413C-81EB-800110419A65}">
-  <dimension ref="A1:K74"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D21:D22"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1588,30 +1668,48 @@
       <c r="C16" t="s">
         <v>64</v>
       </c>
+      <c r="D16" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>64</v>
       </c>
+      <c r="D17" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>64</v>
       </c>
+      <c r="D18" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>64</v>
       </c>
+      <c r="D19" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>64</v>
       </c>
+      <c r="D20" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1902,6 +2000,9 @@
       <c r="C44" t="s">
         <v>77</v>
       </c>
+      <c r="D44" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45">
@@ -1913,6 +2014,9 @@
       <c r="C45" t="s">
         <v>77</v>
       </c>
+      <c r="D45" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
@@ -1924,6 +2028,9 @@
       <c r="C46" t="s">
         <v>77</v>
       </c>
+      <c r="D46" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
@@ -1935,6 +2042,9 @@
       <c r="C47" t="s">
         <v>77</v>
       </c>
+      <c r="D47" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48">
@@ -1946,6 +2056,9 @@
       <c r="C48" t="s">
         <v>77</v>
       </c>
+      <c r="D48" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49">
@@ -1957,6 +2070,9 @@
       <c r="C49" t="s">
         <v>77</v>
       </c>
+      <c r="D49" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50">
@@ -2267,6 +2383,54 @@
       </c>
       <c r="J74" s="1">
         <v>357</v>
+      </c>
+    </row>
+    <row r="75" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C75" t="s">
+        <v>130</v>
+      </c>
+      <c r="D75" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="76" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C76" t="s">
+        <v>130</v>
+      </c>
+      <c r="D76" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="77" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C77" t="s">
+        <v>130</v>
+      </c>
+      <c r="D77" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C78" t="s">
+        <v>130</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="79" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C79" t="s">
+        <v>130</v>
+      </c>
+      <c r="D79" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="80" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C80" t="s">
+        <v>130</v>
+      </c>
+      <c r="D80" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2308,6 +2472,7 @@
     <hyperlink ref="D4" r:id="rId35" xr:uid="{D38CDF7D-9FE1-49F1-A1F8-28032F04F6AB}"/>
     <hyperlink ref="D5" r:id="rId36" xr:uid="{530D22AE-701B-4A32-9512-660098BBDF57}"/>
     <hyperlink ref="D10" r:id="rId37" xr:uid="{A8923910-483F-46D2-8ED9-C10E6AF959E8}"/>
+    <hyperlink ref="D78" r:id="rId38" xr:uid="{DB2F31ED-A20B-4C8C-8687-199BB200EF6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Edits to BB collection procedure
</commit_message>
<xml_diff>
--- a/data/Data Collection.xlsx
+++ b/data/Data Collection.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pconn\OneDrive\Desktop\Data Mining\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CU Boulder - Data Science\Spring 2024\Data Mining\Data_Backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC62B5DB-6473-486F-A05F-BB3AA5397EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8632A504-ECB9-41F3-83C2-D8FB0D9BADB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="1" xr2:uid="{EFA0F3B4-3249-4998-8A76-0DCAF9FCE7B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EFA0F3B4-3249-4998-8A76-0DCAF9FCE7B8}"/>
   </bookViews>
   <sheets>
     <sheet name="productCollectionList" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="206">
   <si>
     <t>id</t>
   </si>
@@ -435,168 +435,310 @@
     <t>bestbuy</t>
   </si>
   <si>
-    <t>https://www.bestbuy.com/site/samsung-galaxy-s23-ultra-256gb-unlocked-phantom-black/6529723.p?skuId=6529723</t>
-  </si>
-  <si>
-    <t>Samsung - Galaxy S23 Ultra 256GB (Unlocked) - Phantom Black</t>
-  </si>
-  <si>
-    <t>https://www.bestbuy.com/site/apple-iphone-13-5g-128gb-unlocked-midnight/6417788.p?skuId=6417788</t>
-  </si>
-  <si>
-    <t>Apple - iPhone 13 5G 128GB (Unlocked) - Midnight</t>
-  </si>
-  <si>
     <t>https://www.bestbuy.com/site/jbl-flip-5-portable-bluetooth-speaker-black/6356535.p?skuId=6356535</t>
   </si>
   <si>
     <t>JBL - Flip 5 Portable Bluetooth Speaker - Black</t>
   </si>
   <si>
-    <t>https://www.bestbuy.com/site/mcafee-total-protection-5-device-antivirus-internet-security-software-1-year-subscription-android-apple-ios-chrome-mac-os-windows-digital/6517326.p?skuId=6517326</t>
-  </si>
-  <si>
-    <t>McAfee - Total Protection (5 Device) Antivirus &amp; Internet Security Software (1-Year Subscription) - Android, Apple iOS, Chrome, Mac OS, Windows [Digital]</t>
-  </si>
-  <si>
-    <t>Real-Time Protection
+    <t>ReviewID</t>
+  </si>
+  <si>
+    <t>review_header</t>
+  </si>
+  <si>
+    <t>reviewer_name</t>
+  </si>
+  <si>
+    <t>review_content</t>
+  </si>
+  <si>
+    <t>review_star_rating</t>
+  </si>
+  <si>
+    <t>review_helpful_votes</t>
+  </si>
+  <si>
+    <t>verified_purchase</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/hp-deskjet-2755e-wireless-all-in-one-color-printer-scanner-copier-with-instant-ink-and-hp-26k67/-/A-82254388</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/jbl-charge-5-portable-bluetooth-waterproof-speaker-red-target-certified-refurbished/-/A-88249290</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/lg-65-34-class-4k-uhd-2160p-smart-oled-tv-oled65c3/-/A-88196023</t>
+  </si>
+  <si>
+    <t>Hogwarts Legacy (XBOX)</t>
+  </si>
+  <si>
+    <t>Jedi Survivor PS5</t>
+  </si>
+  <si>
+    <t>MarioKart8 Deluxe - Switch</t>
+  </si>
+  <si>
+    <t>Ninja Woodfire Pizza Oven</t>
+  </si>
+  <si>
+    <t>Igloo 24qt Cooler</t>
+  </si>
+  <si>
+    <t>Dyson Ball Animal 3 Extra Upright Vacuum Cleaner</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/hogwarts-legacy-xbox-series-x/-/A-86267032</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/star-wars-jedi-survivor-playstation-5/-/A-88183520</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/mario-kart-8-deluxe-nintendo-switch/-/A-52161278</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/ninja-woodfire-pizza-oven-8-in-1-outdoor-oven-5-pizza-settings-smoker-ninja-woodfire-technology-electric-oo101/-/A-89401843</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/igloo-imx-24qt-cooler-meteorite/-/A-87378961</t>
+  </si>
+  <si>
+    <t>https://www.target.com/p/dyson-ball-animal-3-extra-upright-vacuum/-/A-85269264</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Hogwarts-Legacy-Xbox-English-Version-Region/dp/B0B9YSJC5S/ref=sr_1_2?crid=1K69XYMHWNR56&amp;dib=eyJ2IjoiMSJ9.Kg0XV9Kot63z1u2KagkEvpCVUtkbGXvapqAJX7afkiu3BdvCRxuMMxHq3-R-Vq88oqItB-jjTuSzsA4OUT3gHqxnGxm_W3ax9Bt1-kNDhIIrfk2DMuaREs1iW3ZpC41UpXGGXpnKaQWx_QR6PweYu_E0fgQaz6JOeKQrHgmpoGnZNkaPqUf-EzAWuLvi4LuOAF_AT5tsuZUIeboaBcrdGFpzu4TWaNBwkw4WmSvH7Vo.uFmuTgI86APUwJ8qSsprJqvZ4Dnr_EwLXhTo2K61-P0&amp;dib_tag=se&amp;keywords=hogwarts+legacy+xbox&amp;qid=1710278855&amp;sprefix=hogwarts+legacy+xbox%2Caps%2C129&amp;sr=8-2</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Star-Wars-Jedi-Survivor-Playstation-5/dp/B0BPD4JMWT/ref=sr_1_1?crid=1YEWINBQP33M2&amp;dib=eyJ2IjoiMSJ9.xmgn1bEBQh8fF6vN-_ijDTx3NnKfAvuz4KzU8chGgsL67cKZ-GVbOSb0nGWeW8mxQpNntErtqMVDRP2_Qvv6NVonWyAdXrQOG1vF3pQuiK5vfmslLzeTXkEtyMSwY0hE5dvkCY4Udzheb9VLdQgjV4RNjelCbXWMWS3HDuqkxw8RhbOBcyBB1KuJpYwpU0LO3JbTFOrTQoCecarfSPAyc01kEOKHqvHzXAHZPHjTRpo.vqAgJHJ_EuyQ0aHKHSEiLA9mvUUFdQtDGBvQua34gew&amp;dib_tag=se&amp;keywords=jedi+survivor+ps5&amp;qid=1710278950&amp;sprefix=jedi+survivor+ps%2Caps%2C174&amp;sr=8-1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Mario-Kart-8-Deluxe-Nintendo-Switch/dp/B01N1037CV/ref=sr_1_1?crid=1PYFQU1N4B68F&amp;dib=eyJ2IjoiMSJ9.8TZU_Of0o7Vk3YWNjDE9oY9I_W3GMrGxHT454fa05jnyQhIJ1QoKGzaub95DXly85ZIxHf3U7vByBD9UHUHObxJwp-_uYmPTubto19uqmmQglLhYd3W-DOvMZz4lfv1l9ezRsNuuryHtJljvddmeIZdaJWrxpna-VU5FHp3braflTwk_ypjvU7neyKr_vIay2KHtiMOKVjqNxAnzmGjWABX-bq-mvp-ghJ0Hq7eY9h4.vohI6h3tcX_pnwUMLahacLD3yr74bAsNKv9eeH5rAp0&amp;dib_tag=se&amp;keywords=mario+kart+8+deluxe&amp;qid=1710279189&amp;sprefix=mario+kart+%2Caps%2C167&amp;sr=8-1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Ninja-Woodfire-Technology-terracotta-OO101/dp/B0C6BQVDX3/ref=sr_1_3?crid=3DXGBNWLVTJHJ&amp;dib=eyJ2IjoiMSJ9.0WxsIb1exp9JW6Y3VWlsjnd4AbzdLgvTZ3dzGlCYh7z1OEIvxums8Mey72f26ju-BWrkrofq9sMNvCk49njaQbu-SN8ItGFSBFcq-t91Hsb6AE3rPWtoewiMwvt1h2JtkHhsZTKkYeLo0Y9nnD_eJ4STJOza34YIVUe9YB7S8nTqDnhXuTlMQ4TE6pHn3CnUHoVNJGIlgiU2ncUCADPEKpW5C2f1-rC8jpiw7k3qXsE.uqci_nwiB33tgkfGHQRjqPWrYYjoEoVkB-fSO930oYQ&amp;dib_tag=se&amp;keywords=Ninja%2BWoodfire%2BPizza%2BOven%2C%2B8-in-1%2BOutdoor%2BOven&amp;qid=1710280162&amp;sprefix=ninja%2Bwoodfire%2Bpizza%2Boven%2C%2B8-in-1%2Boutdoor%2Boven%2Caps%2C183&amp;sr=8-3&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B08YS7QZLL/ref=twister_B09V6MDSN6?_encoding=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Dyson-Animal-Extra-Upright-Vacuum/dp/B0B57QV5TT/ref=sr_1_3?crid=2IQWXZR08I144&amp;dib=eyJ2IjoiMSJ9.t3iEOoxEJUwLPVoSUcRptqioH5l2EvX8s4APBjqpAjI4e18xB7pmNY8TyLEanhvfvEQqqscP3Xi13oKWZQuQ1MaGTAAh82rbXWBT5nZjBYQqPFp7PUAvYcMk9RslrAyAZS0Nwv3r6RQ8M2iBSK7DQAZmAK0ycSydB1nB1cVDRVBJ0bgIwOtJPiE6ohrQceFbK44RLbkqiNcgSv_YM7QC30n8grFBmSgixz1fAwZtEd8.ZIHRSLxkS_22b7rx1F4ymcSJXsCEuBy_aVi0A1DzCpU&amp;dib_tag=se&amp;keywords=Dyson%2B-%2BBall%2BAnimal%2B3%2BExtra%2BUpright&amp;qid=1710280601&amp;sprefix=dyson%2B-%2Bball%2Banimal%2B3%2Bextra%2Bupright%2Caps%2C176&amp;sr=8-3&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/hogwarts-legacy-standard-edition-xbox-series-x/6502627.p?skuId=6502627</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/star-wars-jedi-survivor-standard-edition-playstation-5/6528657.p?skuId=6528657</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/mario-kart-8-deluxe-nintendo-switch/5723304.p?skuId=5723304</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/igloo-imx-24-quart-cooler-gray/6523836.p?skuId=6523836</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/dyson-ball-animal-3-extra-upright-vacuum-with-5-accessories-copper-silver/6504485.p?skuId=6504485</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/ninja-woodfire-pizza-oven-8-in-1-outdoor-oven-5-pizza-settings-700f-smoker-woodfire-technology-electric-terracotta-red/6548901.p?skuId=6548901</t>
+  </si>
+  <si>
+    <t>Hogwarts Legacy Standard Edition - Xbox Series X</t>
+  </si>
+  <si>
+    <t>Edition Standard Edition
+ESRB Rating T (Teen 13+)
+Compatible Platform(s) Xbox Series X
+Software Format Physical</t>
+  </si>
+  <si>
+    <t>Star Wars Jedi: Survivor Standard Edition - PlayStation 5</t>
+  </si>
+  <si>
+    <t>Edition Standard Edition
+ESRB Rating T (Teen 13+)
+ESRB Descriptors Mild language, Violence
+Compatible Platform(s) PlayStation 5
+Software Format Physical</t>
+  </si>
+  <si>
+    <t>Mario Kart 8 Deluxe - Nintendo Switch</t>
+  </si>
+  <si>
+    <t>ESRB Rating E (Everyone)
+ESRB Descriptors Comic mischief
+Compatible Platform(s) Nintendo Switch
+Software Format Physical</t>
+  </si>
+  <si>
+    <t>Ninja - Woodfire Pizza Oven, 8-in-1 Outdoor Oven, 5 Pizza Settings, 700°F, Smoker, Woodfire Technology, Electric - Terracotta Red</t>
+  </si>
+  <si>
+    <t>Product Name Woodfire Pizza Oven, 8-in-1 Outdoor Oven, 5 Pizza Settings, 700°F, Smoker, Woodfire Technology, Electric
+Brand Ninja
+Model Number OO101
+Color Terracotta Red
+Color Category Red</t>
+  </si>
+  <si>
+    <t>Igloo - IMX 24 Quart Cooler - Gray</t>
+  </si>
+  <si>
+    <t>Hard/Soft Case Hardside
+Capacity 24 quarts
+Product Type Hardside Cooler
+BPA-Free Yes</t>
+  </si>
+  <si>
+    <t>Dyson - Ball Animal 3 Extra Upright Vacuum with 5 accessories - Copper/Silver</t>
+  </si>
+  <si>
+    <t>Pet
 Yes
-E-mail Security
+Cleaning Path Width
+11.02 inches
+Vacuum Type
+Upright vacuums
+Bin Capacity
+0.55 gallons
+Product Weight
+17.33 pounds
+Brush Roll Shut-Off
 Yes
-Parental Controls
-No
-Firewall Type
-Other
-Purchase rights
-Number of Devices
-5</t>
-  </si>
-  <si>
-    <t>https://www.bestbuy.com/site/norton-360-deluxe-5-device-antivirus-internet-security-software-vpn-dark-web-monitoring-1-year-subscription-android-mac-os-windows-apple-ios-digital/6346690.p?skuId=6346690</t>
-  </si>
-  <si>
-    <t>Norton - 360 Deluxe (5 Device) Antivirus Internet Security Software + VPN + Dark Web Monitoring (1 Year Subscription) - Android, Mac OS, Windows, Apple iOS [Digital]</t>
-  </si>
-  <si>
-    <t>Protection Type(s)
-Malware, Password, Phishing, Privacy, Ransomware
-Real-Time Protection
+Bagless
 Yes
-Parental Controls
-Yes
-Firewall Type
-2-way
-In-Software Purchases
-Subscriptions
-Cloud Based Software
-Yes
-Purchase rights
-Number of Devices
-5
-Number of Licenses
-1</t>
-  </si>
-  <si>
-    <t>ReviewID</t>
-  </si>
-  <si>
-    <t>review_header</t>
-  </si>
-  <si>
-    <t>reviewer_name</t>
-  </si>
-  <si>
-    <t>review_content</t>
-  </si>
-  <si>
-    <t>review_star_rating</t>
-  </si>
-  <si>
-    <t>review_helpful_votes</t>
-  </si>
-  <si>
-    <t>verified_purchase</t>
-  </si>
-  <si>
-    <t>https://www.target.com/p/hp-deskjet-2755e-wireless-all-in-one-color-printer-scanner-copier-with-instant-ink-and-hp-26k67/-/A-82254388</t>
-  </si>
-  <si>
-    <t>https://www.target.com/p/jbl-charge-5-portable-bluetooth-waterproof-speaker-red-target-certified-refurbished/-/A-88249290</t>
-  </si>
-  <si>
-    <t>https://www.target.com/p/lg-65-34-class-4k-uhd-2160p-smart-oled-tv-oled65c3/-/A-88196023</t>
-  </si>
-  <si>
-    <t>Hogwarts Legacy (XBOX)</t>
-  </si>
-  <si>
-    <t>Jedi Survivor PS5</t>
-  </si>
-  <si>
-    <t>MarioKart8 Deluxe - Switch</t>
-  </si>
-  <si>
-    <t>Ninja Woodfire Pizza Oven</t>
-  </si>
-  <si>
-    <t>Igloo 24qt Cooler</t>
-  </si>
-  <si>
-    <t>Dyson Ball Animal 3 Extra Upright Vacuum Cleaner</t>
-  </si>
-  <si>
-    <t>https://www.target.com/p/hogwarts-legacy-xbox-series-x/-/A-86267032</t>
-  </si>
-  <si>
-    <t>https://www.target.com/p/star-wars-jedi-survivor-playstation-5/-/A-88183520</t>
-  </si>
-  <si>
-    <t>https://www.target.com/p/mario-kart-8-deluxe-nintendo-switch/-/A-52161278</t>
-  </si>
-  <si>
-    <t>https://www.target.com/p/ninja-woodfire-pizza-oven-8-in-1-outdoor-oven-5-pizza-settings-smoker-ninja-woodfire-technology-electric-oo101/-/A-89401843</t>
-  </si>
-  <si>
-    <t>https://www.target.com/p/igloo-imx-24qt-cooler-meteorite/-/A-87378961</t>
-  </si>
-  <si>
-    <t>https://www.target.com/p/dyson-ball-animal-3-extra-upright-vacuum/-/A-85269264</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Hogwarts-Legacy-Xbox-English-Version-Region/dp/B0B9YSJC5S/ref=sr_1_2?crid=1K69XYMHWNR56&amp;dib=eyJ2IjoiMSJ9.Kg0XV9Kot63z1u2KagkEvpCVUtkbGXvapqAJX7afkiu3BdvCRxuMMxHq3-R-Vq88oqItB-jjTuSzsA4OUT3gHqxnGxm_W3ax9Bt1-kNDhIIrfk2DMuaREs1iW3ZpC41UpXGGXpnKaQWx_QR6PweYu_E0fgQaz6JOeKQrHgmpoGnZNkaPqUf-EzAWuLvi4LuOAF_AT5tsuZUIeboaBcrdGFpzu4TWaNBwkw4WmSvH7Vo.uFmuTgI86APUwJ8qSsprJqvZ4Dnr_EwLXhTo2K61-P0&amp;dib_tag=se&amp;keywords=hogwarts+legacy+xbox&amp;qid=1710278855&amp;sprefix=hogwarts+legacy+xbox%2Caps%2C129&amp;sr=8-2</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Star-Wars-Jedi-Survivor-Playstation-5/dp/B0BPD4JMWT/ref=sr_1_1?crid=1YEWINBQP33M2&amp;dib=eyJ2IjoiMSJ9.xmgn1bEBQh8fF6vN-_ijDTx3NnKfAvuz4KzU8chGgsL67cKZ-GVbOSb0nGWeW8mxQpNntErtqMVDRP2_Qvv6NVonWyAdXrQOG1vF3pQuiK5vfmslLzeTXkEtyMSwY0hE5dvkCY4Udzheb9VLdQgjV4RNjelCbXWMWS3HDuqkxw8RhbOBcyBB1KuJpYwpU0LO3JbTFOrTQoCecarfSPAyc01kEOKHqvHzXAHZPHjTRpo.vqAgJHJ_EuyQ0aHKHSEiLA9mvUUFdQtDGBvQua34gew&amp;dib_tag=se&amp;keywords=jedi+survivor+ps5&amp;qid=1710278950&amp;sprefix=jedi+survivor+ps%2Caps%2C174&amp;sr=8-1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Mario-Kart-8-Deluxe-Nintendo-Switch/dp/B01N1037CV/ref=sr_1_1?crid=1PYFQU1N4B68F&amp;dib=eyJ2IjoiMSJ9.8TZU_Of0o7Vk3YWNjDE9oY9I_W3GMrGxHT454fa05jnyQhIJ1QoKGzaub95DXly85ZIxHf3U7vByBD9UHUHObxJwp-_uYmPTubto19uqmmQglLhYd3W-DOvMZz4lfv1l9ezRsNuuryHtJljvddmeIZdaJWrxpna-VU5FHp3braflTwk_ypjvU7neyKr_vIay2KHtiMOKVjqNxAnzmGjWABX-bq-mvp-ghJ0Hq7eY9h4.vohI6h3tcX_pnwUMLahacLD3yr74bAsNKv9eeH5rAp0&amp;dib_tag=se&amp;keywords=mario+kart+8+deluxe&amp;qid=1710279189&amp;sprefix=mario+kart+%2Caps%2C167&amp;sr=8-1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Ninja-Woodfire-Technology-terracotta-OO101/dp/B0C6BQVDX3/ref=sr_1_3?crid=3DXGBNWLVTJHJ&amp;dib=eyJ2IjoiMSJ9.0WxsIb1exp9JW6Y3VWlsjnd4AbzdLgvTZ3dzGlCYh7z1OEIvxums8Mey72f26ju-BWrkrofq9sMNvCk49njaQbu-SN8ItGFSBFcq-t91Hsb6AE3rPWtoewiMwvt1h2JtkHhsZTKkYeLo0Y9nnD_eJ4STJOza34YIVUe9YB7S8nTqDnhXuTlMQ4TE6pHn3CnUHoVNJGIlgiU2ncUCADPEKpW5C2f1-rC8jpiw7k3qXsE.uqci_nwiB33tgkfGHQRjqPWrYYjoEoVkB-fSO930oYQ&amp;dib_tag=se&amp;keywords=Ninja%2BWoodfire%2BPizza%2BOven%2C%2B8-in-1%2BOutdoor%2BOven&amp;qid=1710280162&amp;sprefix=ninja%2Bwoodfire%2Bpizza%2Boven%2C%2B8-in-1%2Boutdoor%2Boven%2Caps%2C183&amp;sr=8-3&amp;th=1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/dp/B08YS7QZLL/ref=twister_B09V6MDSN6?_encoding=UTF8&amp;psc=1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Dyson-Animal-Extra-Upright-Vacuum/dp/B0B57QV5TT/ref=sr_1_3?crid=2IQWXZR08I144&amp;dib=eyJ2IjoiMSJ9.t3iEOoxEJUwLPVoSUcRptqioH5l2EvX8s4APBjqpAjI4e18xB7pmNY8TyLEanhvfvEQqqscP3Xi13oKWZQuQ1MaGTAAh82rbXWBT5nZjBYQqPFp7PUAvYcMk9RslrAyAZS0Nwv3r6RQ8M2iBSK7DQAZmAK0ycSydB1nB1cVDRVBJ0bgIwOtJPiE6ohrQceFbK44RLbkqiNcgSv_YM7QC30n8grFBmSgixz1fAwZtEd8.ZIHRSLxkS_22b7rx1F4ymcSJXsCEuBy_aVi0A1DzCpU&amp;dib_tag=se&amp;keywords=Dyson%2B-%2BBall%2BAnimal%2B3%2BExtra%2BUpright&amp;qid=1710280601&amp;sprefix=dyson%2B-%2Bball%2Banimal%2B3%2Bextra%2Bupright%2Caps%2C176&amp;sr=8-3&amp;th=1</t>
-  </si>
-  <si>
-    <t>https://www.bestbuy.com/site/hogwarts-legacy-standard-edition-xbox-series-x/6502627.p?skuId=6502627</t>
-  </si>
-  <si>
-    <t>https://www.bestbuy.com/site/star-wars-jedi-survivor-standard-edition-playstation-5/6528657.p?skuId=6528657</t>
-  </si>
-  <si>
-    <t>https://www.bestbuy.com/site/mario-kart-8-deluxe-nintendo-switch/5723304.p?skuId=5723304</t>
-  </si>
-  <si>
-    <t>https://www.bestbuy.com/site/igloo-imx-24-quart-cooler-gray/6523836.p?skuId=6523836</t>
-  </si>
-  <si>
-    <t>https://www.bestbuy.com/site/dyson-ball-animal-3-extra-upright-vacuum-with-5-accessories-copper-silver/6504485.p?skuId=6504485</t>
-  </si>
-  <si>
-    <t>https://www.bestbuy.com/site/ninja-woodfire-pizza-oven-8-in-1-outdoor-oven-5-pizza-settings-700f-smoker-woodfire-technology-electric-terracotta-red/6548901.p?skuId=6548901</t>
+Compatible Floor Type
+All floors
+Amperage
+11.67 amperes
+Corded/Cordless
+Corded
+Carpet Height Adjustments Yes
+Wattage 1400 watts
+Wet And Dry Usage No
+Cord Length 35 feet
+Filter Type Lifetime
+Hypoallergenic Yes
+Multi Surface Yes
+Washable Filter Yes
+Attachments Included Combination tool, Stair tool, Tangle-free turbine tool, groom tool, Tool holder</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/ge-1-4-cu-ft-mid-size-microwave-black/3180025.p?skuId=3180025</t>
+  </si>
+  <si>
+    <t>GE - 1.4 Cu. Ft. Mid-Size Microwave - Black</t>
+  </si>
+  <si>
+    <t>Product Height
+12 1/2 inches
+Product Width 21 7/8 inches
+Product Depth 16 3/8 inches
+App Compatible No
+Microwave Type Countertop
+Turntable Diameter 12 5/8 inches</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/lg-65-class-c3-series-oled-4k-uhd-smart-webos-tv/6535929.p?skuId=6535929</t>
+  </si>
+  <si>
+    <t>LG - 65" Class C3 Series OLED 4K UHD Smart webOS TV</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/razor-mx350-dirt-rocket-ebike-w-7-miles-max-operating-range-14-mph-max-speed-small-blue/3698469.p?skuId=3698469</t>
+  </si>
+  <si>
+    <t>Razor - MX350 Dirt Rocket eBike w/7 miles Max Operating Range &amp; 14 mph Max Speed - Small - Blue</t>
+  </si>
+  <si>
+    <t>Product Weight 62.7 pounds
+Battery Charge Time 12 hours
+Battery Voltage 12 volts
+Maximum Operating Range 7 miles
+Maximum Speed 14 miles per hour
+Electric Bike Classification Class 3</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/hamilton-beach-classic-4-slice-toaster-with-sure-toast-technology-stainless-steel/6518125.p?skuId=6518125</t>
+  </si>
+  <si>
+    <t>Hamilton Beach - Classic 4 Slice Toaster with Sure-Toast Technology - Stainless Steel</t>
+  </si>
+  <si>
+    <t>Function(s)
+Bagel, Defrost, Toast, Pastry, Waffle
+Number of Toasting Slots
+4</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/turbotax-deluxe-2023-federal-e-file-state-mac-os-windows-digital/6560825.p?skuId=6560825</t>
+  </si>
+  <si>
+    <t>TurboTax - Deluxe 2023 Federal + E-file &amp; State - Mac OS, Windows [Digital]</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/microsoft-365-family-up-to-6-people-12-month-subscription-activation-required-windows-mac-os-apple-ios-android-digital/6258038.p?skuId=6258038</t>
+  </si>
+  <si>
+    <t>Microsoft - 365 Family (Up to 6 People) (12-Month Subscription) - Activation Required - Windows, Mac OS, Apple iOS, Android [Digital]</t>
+  </si>
+  <si>
+    <t>Number of Users 1
+Number of Licenses 1
+Operating System Compatibility Mac OS, Windows
+Software Format Digital</t>
+  </si>
+  <si>
+    <t>Number of Users 6
+Number of Devices 5
+Number of Licenses 1
+Operating System Compatibility Windows, Mac OS, Apple iOS, Android
+Software Format Digital
+Subscription Period 1 Year</t>
+  </si>
+  <si>
+    <t>Wireless Yes
+Connectivity Technology Bluetooth
+Rechargeable Yes
+Battery Life 12 hours
+USB Device Charging Yes</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/hp-deskjet-2755e-wireless-inkjet-printer-with-3-months-of-instant-ink-included-with-hp-white/6454282.p?skuId=6454282</t>
+  </si>
+  <si>
+    <t>HP - DeskJet 2755e Wireless Inkjet Printer with 3 months of Instant Ink Included with HP+ - White</t>
+  </si>
+  <si>
+    <t>Mobile Device Printing Yes
+Networking Wireless
+ENERGY STAR Certified Yes
+Printer Type Printer, Scanner, Copier
+ISO Color Print Speed 5.5 pages per minute
+ISO Mono Print Speed 7.5 pages per minute</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/samsung-galaxy-s22-ultra-128gb-phantom-black-verizon/6494471.p?skuId=6494471</t>
+  </si>
+  <si>
+    <t>Samsung - Galaxy S22 Ultra 128GB - Phantom Black (Verizon)</t>
+  </si>
+  <si>
+    <t>Screen Size 6.8 inches
+Front-Facing Camera 40 megapixels
+Rear-Facing Camera 108 megapixels
+Series Galaxy S22</t>
+  </si>
+  <si>
+    <t>https://www.bestbuy.com/site/apple-iphone-14-128gb-unlocked-midnight/6507555.p?skuId=6507555</t>
+  </si>
+  <si>
+    <t>Apple - iPhone 14 128GB (Unlocked) - Midnight</t>
+  </si>
+  <si>
+    <t>Screen Size 6.1 inches
+Front-Facing Camera 12 megapixels
+Rear-Facing Camera 12 megapixels</t>
   </si>
 </sst>
 </file>
@@ -1017,18 +1159,18 @@
   <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" customWidth="1"/>
-    <col min="4" max="4" width="47.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1040,7 +1182,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1052,7 +1194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1062,7 +1204,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1074,7 +1216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1086,7 +1228,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1098,7 +1240,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1110,7 +1252,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1122,7 +1264,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1134,7 +1276,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1146,7 +1288,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1158,7 +1300,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1168,7 +1310,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -1180,7 +1322,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1192,7 +1334,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1206,75 +1348,75 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
         <v>32</v>
       </c>
@@ -1282,7 +1424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
         <v>33</v>
       </c>
@@ -1290,31 +1432,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="D45" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="D46" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="D47" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="D48" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>38</v>
       </c>
@@ -1322,7 +1464,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>8</v>
       </c>
@@ -1330,19 +1472,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="D51" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="D52" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>40</v>
       </c>
@@ -1350,7 +1492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>41</v>
       </c>
@@ -1358,25 +1500,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
       <c r="D59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
         <v>43</v>
       </c>
@@ -1384,19 +1526,19 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
       <c r="D61" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
       <c r="D62" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
         <v>45</v>
       </c>
@@ -1404,7 +1546,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
         <v>47</v>
       </c>
@@ -1412,12 +1554,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
         <v>49</v>
       </c>
@@ -1425,7 +1567,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
         <v>51</v>
       </c>
@@ -1433,7 +1575,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>52</v>
       </c>
@@ -1453,26 +1595,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8FFCC8-FB4D-413C-81EB-800110419A65}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.54296875" customWidth="1"/>
-    <col min="4" max="4" width="98.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.1796875" customWidth="1"/>
-    <col min="6" max="6" width="29.7265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.81640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.81640625" customWidth="1"/>
-    <col min="11" max="11" width="22.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="98.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1482,7 +1624,7 @@
       <c r="C1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1504,7 +1646,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1514,245 +1656,245 @@
       <c r="C2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>150</v>
+      <c r="D4" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>151</v>
+      <c r="D5" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>68</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>69</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>70</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>152</v>
+      <c r="D10" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>72</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>73</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>74</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>75</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>64</v>
       </c>
-      <c r="D16" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D16" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>64</v>
       </c>
-      <c r="D17" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D17" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>64</v>
       </c>
-      <c r="D18" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D18" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>64</v>
       </c>
-      <c r="D19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D19" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>64</v>
       </c>
-      <c r="D20" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D20" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>64</v>
       </c>
-      <c r="D21" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D21" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1762,14 +1904,14 @@
       <c r="C30" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="3" t="s">
         <v>78</v>
       </c>
       <c r="E30" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1779,14 +1921,14 @@
       <c r="C31" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1796,14 +1938,14 @@
       <c r="C32" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1813,14 +1955,14 @@
       <c r="C33" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5</v>
       </c>
@@ -1830,14 +1972,14 @@
       <c r="C34" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>6</v>
       </c>
@@ -1847,14 +1989,14 @@
       <c r="C35" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="3" t="s">
         <v>89</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7</v>
       </c>
@@ -1864,14 +2006,14 @@
       <c r="C36" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8</v>
       </c>
@@ -1881,14 +2023,14 @@
       <c r="C37" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="3" t="s">
         <v>93</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9</v>
       </c>
@@ -1898,14 +2040,14 @@
       <c r="C38" t="s">
         <v>77</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="3" t="s">
         <v>95</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>10</v>
       </c>
@@ -1915,14 +2057,14 @@
       <c r="C39" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="3" t="s">
         <v>97</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>11</v>
       </c>
@@ -1932,14 +2074,14 @@
       <c r="C40" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="3" t="s">
         <v>99</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>12</v>
       </c>
@@ -1949,14 +2091,14 @@
       <c r="C41" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="3" t="s">
         <v>101</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>13</v>
       </c>
@@ -1966,14 +2108,14 @@
       <c r="C42" t="s">
         <v>77</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="3" t="s">
         <v>103</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>14</v>
       </c>
@@ -1983,14 +2125,14 @@
       <c r="C43" t="s">
         <v>77</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="3" t="s">
         <v>105</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>15</v>
       </c>
@@ -2000,11 +2142,11 @@
       <c r="C44" t="s">
         <v>77</v>
       </c>
-      <c r="D44" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D44" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>16</v>
       </c>
@@ -2014,11 +2156,11 @@
       <c r="C45" t="s">
         <v>77</v>
       </c>
-      <c r="D45" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D45" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>17</v>
       </c>
@@ -2028,11 +2170,11 @@
       <c r="C46" t="s">
         <v>77</v>
       </c>
-      <c r="D46" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D46" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>18</v>
       </c>
@@ -2042,11 +2184,11 @@
       <c r="C47" t="s">
         <v>77</v>
       </c>
-      <c r="D47" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D47" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>19</v>
       </c>
@@ -2056,11 +2198,11 @@
       <c r="C48" t="s">
         <v>77</v>
       </c>
-      <c r="D48" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D48" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>20</v>
       </c>
@@ -2070,11 +2212,11 @@
       <c r="C49" t="s">
         <v>77</v>
       </c>
-      <c r="D49" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D49" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>21</v>
       </c>
@@ -2085,7 +2227,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>22</v>
       </c>
@@ -2096,7 +2238,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>23</v>
       </c>
@@ -2107,7 +2249,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>24</v>
       </c>
@@ -2118,7 +2260,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>25</v>
       </c>
@@ -2129,7 +2271,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>26</v>
       </c>
@@ -2140,7 +2282,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>27</v>
       </c>
@@ -2150,7 +2292,7 @@
       <c r="C56" t="s">
         <v>77</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="3" t="s">
         <v>119</v>
       </c>
       <c r="E56" s="2"/>
@@ -2164,7 +2306,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>28</v>
       </c>
@@ -2174,7 +2316,7 @@
       <c r="C57" t="s">
         <v>77</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="3" t="s">
         <v>122</v>
       </c>
       <c r="E57" s="2"/>
@@ -2188,7 +2330,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>29</v>
       </c>
@@ -2198,7 +2340,7 @@
       <c r="C58" t="s">
         <v>77</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="3" t="s">
         <v>125</v>
       </c>
       <c r="E58" s="2"/>
@@ -2212,7 +2354,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>30</v>
       </c>
@@ -2222,7 +2364,7 @@
       <c r="C59" t="s">
         <v>77</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="3" t="s">
         <v>128</v>
       </c>
       <c r="E59" s="2"/>
@@ -2236,243 +2378,447 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:11" ht="60" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D65" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I65" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J65">
+        <v>211</v>
+      </c>
+      <c r="K65">
+        <v>729.99</v>
+      </c>
+    </row>
+    <row r="66" spans="3:11" ht="90" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="67" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D66" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I66" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J66">
+        <v>396</v>
+      </c>
+      <c r="K66">
+        <v>1199.99</v>
+      </c>
+    </row>
+    <row r="67" spans="3:11" ht="135" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D67" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I67" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J67">
+        <v>3496</v>
+      </c>
+      <c r="K67">
+        <v>49.99</v>
+      </c>
+    </row>
+    <row r="68" spans="3:11" ht="75" x14ac:dyDescent="0.25">
       <c r="C68" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D68" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I68" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="J68">
+        <v>5938</v>
+      </c>
+      <c r="K68">
+        <v>89.99</v>
+      </c>
+    </row>
+    <row r="69" spans="3:11" ht="120" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>130</v>
       </c>
-      <c r="D69" s="1"/>
+      <c r="D69" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="E69" s="1"/>
-      <c r="J69" s="1"/>
-    </row>
-    <row r="70" spans="3:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="F69" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I69" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="J69" s="1">
+        <v>10362</v>
+      </c>
+      <c r="K69">
+        <v>99.99</v>
+      </c>
+    </row>
+    <row r="70" spans="3:11" ht="75" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>130</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>131</v>
+        <v>190</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="1" t="s">
-        <v>132</v>
+        <v>191</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="I70" s="1">
-        <v>4.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="J70" s="1">
-        <v>2052</v>
-      </c>
-    </row>
-    <row r="71" spans="3:10" ht="29" x14ac:dyDescent="0.35">
+        <v>315</v>
+      </c>
+      <c r="K70">
+        <v>69.989999999999995</v>
+      </c>
+    </row>
+    <row r="71" spans="3:11" ht="60" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>130</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>133</v>
+        <v>187</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="1" t="s">
-        <v>134</v>
+        <v>188</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="I71" s="1">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="J71" s="1">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="72" spans="3:10" ht="29" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="K71">
+        <v>49.99</v>
+      </c>
+    </row>
+    <row r="72" spans="3:11" ht="90" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>130</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="1" t="s">
-        <v>136</v>
+        <v>185</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="I72" s="1">
-        <v>4.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="J72" s="1">
-        <v>5921</v>
-      </c>
-    </row>
-    <row r="73" spans="3:10" ht="159.5" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+      <c r="K72">
+        <v>339.99</v>
+      </c>
+    </row>
+    <row r="73" spans="3:11" ht="30" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>130</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>137</v>
+        <v>182</v>
       </c>
       <c r="E73" s="3"/>
       <c r="F73" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>139</v>
+        <v>183</v>
       </c>
       <c r="I73" s="1">
-        <v>4.5999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="J73" s="1">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="74" spans="3:10" ht="261" x14ac:dyDescent="0.35">
+        <v>1499</v>
+      </c>
+      <c r="K73">
+        <v>1599.99</v>
+      </c>
+    </row>
+    <row r="74" spans="3:11" ht="105" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
         <v>130</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="1" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="I74" s="1">
-        <v>4.4000000000000004</v>
+        <v>4</v>
       </c>
       <c r="J74" s="1">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="75" spans="3:10" x14ac:dyDescent="0.35">
+        <v>860</v>
+      </c>
+      <c r="K74">
+        <v>139.99</v>
+      </c>
+    </row>
+    <row r="75" spans="3:11" ht="75" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>130</v>
       </c>
-      <c r="D75" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="76" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D75" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I75" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="J75" s="1">
+        <v>380</v>
+      </c>
+      <c r="K75">
+        <v>44.99</v>
+      </c>
+    </row>
+    <row r="76" spans="3:11" ht="105" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
         <v>130</v>
       </c>
-      <c r="D76" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="77" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D76" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I76" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="J76" s="1">
+        <v>1527</v>
+      </c>
+      <c r="K76">
+        <v>34.99</v>
+      </c>
+    </row>
+    <row r="77" spans="3:11" ht="75" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
         <v>130</v>
       </c>
-      <c r="D77" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D77" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I77" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J77" s="1">
+        <v>32562</v>
+      </c>
+      <c r="K77">
+        <v>39.99</v>
+      </c>
+    </row>
+    <row r="78" spans="3:11" ht="120" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>130</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="79" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D78" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I78" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="J78" s="1">
+        <v>106</v>
+      </c>
+      <c r="K78">
+        <v>349.99</v>
+      </c>
+    </row>
+    <row r="79" spans="3:11" ht="60" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
         <v>130</v>
       </c>
-      <c r="D79" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="80" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D79" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I79" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J79" s="1">
+        <v>41</v>
+      </c>
+      <c r="K79">
+        <v>94.99</v>
+      </c>
+    </row>
+    <row r="80" spans="3:11" ht="409.5" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
         <v>130</v>
       </c>
-      <c r="D80" t="s">
-        <v>175</v>
+      <c r="D80" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I80" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J80" s="1">
+        <v>777</v>
+      </c>
+      <c r="K80">
+        <v>399.99</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D73" r:id="rId1" xr:uid="{811ED660-001E-4E8A-80C6-728534F9A173}"/>
-    <hyperlink ref="D74" r:id="rId2" xr:uid="{DEDC594A-A2C7-4F66-A7E5-6D8DFEA9E67F}"/>
-    <hyperlink ref="D72" r:id="rId3" xr:uid="{54C98A58-57BD-4CEC-BDB6-9D43620C9C0D}"/>
-    <hyperlink ref="D71" r:id="rId4" xr:uid="{5555D41F-F7F8-4B34-9976-EEE0691A5EC9}"/>
-    <hyperlink ref="D70" r:id="rId5" xr:uid="{3EE01161-EC61-4EEB-8749-06092492123A}"/>
-    <hyperlink ref="D30" r:id="rId6" xr:uid="{130ED931-C0D5-4631-8A44-4F9CED526F3D}"/>
-    <hyperlink ref="D31" r:id="rId7" xr:uid="{A76F5837-6645-4380-8C05-A032935932AA}"/>
-    <hyperlink ref="D32" r:id="rId8" xr:uid="{F4B38194-9784-42C6-B5FB-5DC0352BF3BC}"/>
-    <hyperlink ref="D33" r:id="rId9" xr:uid="{8EB8E547-29B8-4034-BC7A-1E38C13302F7}"/>
-    <hyperlink ref="D34" r:id="rId10" xr:uid="{D3B90A15-B487-4718-B67A-D9A783549002}"/>
-    <hyperlink ref="D35" r:id="rId11" xr:uid="{9240A67F-E936-4A7A-B8DD-99B93704DFD3}"/>
-    <hyperlink ref="D36" r:id="rId12" xr:uid="{15A49671-BF18-4C6B-8525-B693F179BD7A}"/>
-    <hyperlink ref="D37" r:id="rId13" xr:uid="{6221B301-6B94-46CC-8728-319A961E1C22}"/>
-    <hyperlink ref="D38" r:id="rId14" xr:uid="{0EA6C536-7C11-4E3B-A72C-D044F33EDC31}"/>
-    <hyperlink ref="D39" r:id="rId15" xr:uid="{EE7EB3A1-A27F-4709-AEEC-F8067DA82420}"/>
-    <hyperlink ref="D40" r:id="rId16" xr:uid="{68263586-9729-4689-A0D1-406BD38D45D8}"/>
-    <hyperlink ref="D41" r:id="rId17" xr:uid="{CA9189C5-F2CE-48A8-AAF3-BBE8517CE44B}"/>
-    <hyperlink ref="D42" r:id="rId18" xr:uid="{C44812AC-BA35-4E7E-8174-CAE21A17EAAE}"/>
-    <hyperlink ref="D43" r:id="rId19" xr:uid="{6276CFCE-9952-42A8-BA0A-B30C727BE342}"/>
-    <hyperlink ref="D56" r:id="rId20" xr:uid="{911155BB-A88A-4C90-A863-325DCD0E385B}"/>
-    <hyperlink ref="D57" r:id="rId21" xr:uid="{445282CD-8591-4C05-BE45-9FDE0FC92D35}"/>
-    <hyperlink ref="D58" r:id="rId22" xr:uid="{FBBAEFD8-1EA7-4308-A8DB-5B363FDE6573}"/>
-    <hyperlink ref="D59" r:id="rId23" xr:uid="{0D5F9383-36E8-4E03-BE21-427ED2729086}"/>
-    <hyperlink ref="D2" r:id="rId24" xr:uid="{CAD9AB78-FE3F-45E3-A8C4-3091ADF185E8}"/>
-    <hyperlink ref="D3" r:id="rId25" xr:uid="{0590ADB1-8931-47E6-A9F9-635B5C713D11}"/>
-    <hyperlink ref="D6" r:id="rId26" xr:uid="{8E2BE472-0220-4AFC-8868-DD61E717ED8A}"/>
-    <hyperlink ref="D7" r:id="rId27" xr:uid="{A2F21B63-6932-487D-8998-597425811A48}"/>
-    <hyperlink ref="D8" r:id="rId28" xr:uid="{79C1DC41-5DBC-4BDB-BDF0-84E81FA68FA1}"/>
-    <hyperlink ref="D9" r:id="rId29" xr:uid="{1EBCD253-DB99-4828-A82C-95E26C544FCB}"/>
-    <hyperlink ref="D11" r:id="rId30" xr:uid="{DB4CBE25-561E-4694-B7E1-01D96706296F}"/>
-    <hyperlink ref="D14" r:id="rId31" xr:uid="{09675619-C1DA-4BC4-A080-53E08339B896}"/>
-    <hyperlink ref="D15" r:id="rId32" xr:uid="{1CD5ED3E-0215-488D-8CF9-29EE2B7F29F6}"/>
-    <hyperlink ref="D12" r:id="rId33" xr:uid="{F5BD0E9E-68D4-4B40-A9D0-59034348797F}"/>
-    <hyperlink ref="D13" r:id="rId34" xr:uid="{61558A01-8BE8-49DB-8FDF-7949BD05D0CA}"/>
-    <hyperlink ref="D4" r:id="rId35" xr:uid="{D38CDF7D-9FE1-49F1-A1F8-28032F04F6AB}"/>
-    <hyperlink ref="D5" r:id="rId36" xr:uid="{530D22AE-701B-4A32-9512-660098BBDF57}"/>
-    <hyperlink ref="D10" r:id="rId37" xr:uid="{A8923910-483F-46D2-8ED9-C10E6AF959E8}"/>
-    <hyperlink ref="D78" r:id="rId38" xr:uid="{DB2F31ED-A20B-4C8C-8687-199BB200EF6C}"/>
+    <hyperlink ref="D30" r:id="rId1" xr:uid="{130ED931-C0D5-4631-8A44-4F9CED526F3D}"/>
+    <hyperlink ref="D31" r:id="rId2" xr:uid="{A76F5837-6645-4380-8C05-A032935932AA}"/>
+    <hyperlink ref="D32" r:id="rId3" xr:uid="{F4B38194-9784-42C6-B5FB-5DC0352BF3BC}"/>
+    <hyperlink ref="D33" r:id="rId4" xr:uid="{8EB8E547-29B8-4034-BC7A-1E38C13302F7}"/>
+    <hyperlink ref="D34" r:id="rId5" xr:uid="{D3B90A15-B487-4718-B67A-D9A783549002}"/>
+    <hyperlink ref="D35" r:id="rId6" xr:uid="{9240A67F-E936-4A7A-B8DD-99B93704DFD3}"/>
+    <hyperlink ref="D36" r:id="rId7" xr:uid="{15A49671-BF18-4C6B-8525-B693F179BD7A}"/>
+    <hyperlink ref="D37" r:id="rId8" xr:uid="{6221B301-6B94-46CC-8728-319A961E1C22}"/>
+    <hyperlink ref="D38" r:id="rId9" xr:uid="{0EA6C536-7C11-4E3B-A72C-D044F33EDC31}"/>
+    <hyperlink ref="D39" r:id="rId10" xr:uid="{EE7EB3A1-A27F-4709-AEEC-F8067DA82420}"/>
+    <hyperlink ref="D40" r:id="rId11" xr:uid="{68263586-9729-4689-A0D1-406BD38D45D8}"/>
+    <hyperlink ref="D41" r:id="rId12" xr:uid="{CA9189C5-F2CE-48A8-AAF3-BBE8517CE44B}"/>
+    <hyperlink ref="D42" r:id="rId13" xr:uid="{C44812AC-BA35-4E7E-8174-CAE21A17EAAE}"/>
+    <hyperlink ref="D43" r:id="rId14" xr:uid="{6276CFCE-9952-42A8-BA0A-B30C727BE342}"/>
+    <hyperlink ref="D56" r:id="rId15" xr:uid="{911155BB-A88A-4C90-A863-325DCD0E385B}"/>
+    <hyperlink ref="D57" r:id="rId16" xr:uid="{445282CD-8591-4C05-BE45-9FDE0FC92D35}"/>
+    <hyperlink ref="D58" r:id="rId17" xr:uid="{FBBAEFD8-1EA7-4308-A8DB-5B363FDE6573}"/>
+    <hyperlink ref="D59" r:id="rId18" xr:uid="{0D5F9383-36E8-4E03-BE21-427ED2729086}"/>
+    <hyperlink ref="D2" r:id="rId19" xr:uid="{CAD9AB78-FE3F-45E3-A8C4-3091ADF185E8}"/>
+    <hyperlink ref="D3" r:id="rId20" xr:uid="{0590ADB1-8931-47E6-A9F9-635B5C713D11}"/>
+    <hyperlink ref="D6" r:id="rId21" xr:uid="{8E2BE472-0220-4AFC-8868-DD61E717ED8A}"/>
+    <hyperlink ref="D7" r:id="rId22" xr:uid="{A2F21B63-6932-487D-8998-597425811A48}"/>
+    <hyperlink ref="D8" r:id="rId23" xr:uid="{79C1DC41-5DBC-4BDB-BDF0-84E81FA68FA1}"/>
+    <hyperlink ref="D9" r:id="rId24" xr:uid="{1EBCD253-DB99-4828-A82C-95E26C544FCB}"/>
+    <hyperlink ref="D11" r:id="rId25" xr:uid="{DB4CBE25-561E-4694-B7E1-01D96706296F}"/>
+    <hyperlink ref="D14" r:id="rId26" xr:uid="{09675619-C1DA-4BC4-A080-53E08339B896}"/>
+    <hyperlink ref="D15" r:id="rId27" xr:uid="{1CD5ED3E-0215-488D-8CF9-29EE2B7F29F6}"/>
+    <hyperlink ref="D12" r:id="rId28" xr:uid="{F5BD0E9E-68D4-4B40-A9D0-59034348797F}"/>
+    <hyperlink ref="D13" r:id="rId29" xr:uid="{61558A01-8BE8-49DB-8FDF-7949BD05D0CA}"/>
+    <hyperlink ref="D4" r:id="rId30" xr:uid="{D38CDF7D-9FE1-49F1-A1F8-28032F04F6AB}"/>
+    <hyperlink ref="D5" r:id="rId31" xr:uid="{530D22AE-701B-4A32-9512-660098BBDF57}"/>
+    <hyperlink ref="D10" r:id="rId32" xr:uid="{A8923910-483F-46D2-8ED9-C10E6AF959E8}"/>
+    <hyperlink ref="D78" r:id="rId33" xr:uid="{DB2F31ED-A20B-4C8C-8687-199BB200EF6C}"/>
+    <hyperlink ref="D75" r:id="rId34" xr:uid="{7D001425-952B-4273-9E9A-FCE3CB5FFF9A}"/>
+    <hyperlink ref="D76" r:id="rId35" xr:uid="{156ECCF7-0BD4-43A9-B176-59C6D564886B}"/>
+    <hyperlink ref="D77" r:id="rId36" xr:uid="{918848D8-7BE5-4018-8C55-CEC7002CA9F2}"/>
+    <hyperlink ref="D79" r:id="rId37" xr:uid="{8E1E973E-3ACA-4E7C-AD67-B499DA21FEA1}"/>
+    <hyperlink ref="D80" r:id="rId38" xr:uid="{4FD46094-DAB9-4CD6-A190-C0C6227810FC}"/>
+    <hyperlink ref="D69" r:id="rId39" xr:uid="{7716567D-D933-48C2-9224-35CA8B300709}"/>
+    <hyperlink ref="D68" r:id="rId40" xr:uid="{6E2FCDC0-D3E2-4E28-9D42-F1F93D03797C}"/>
+    <hyperlink ref="D67" r:id="rId41" xr:uid="{417AACA0-6100-426E-85C1-0AF8CC02E529}"/>
+    <hyperlink ref="D66" r:id="rId42" xr:uid="{DAC37E6D-5373-4CEA-BF1C-8C46D88AC0DF}"/>
+    <hyperlink ref="D65" r:id="rId43" xr:uid="{1FD7B0EC-16E0-4C60-AE94-7B4720546328}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2487,19 +2833,19 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -2507,25 +2853,25 @@
         <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="F1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="G1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="H1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="I1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data Collection table updated; Desc added to data.qmd
</commit_message>
<xml_diff>
--- a/data/Data Collection.xlsx
+++ b/data/Data Collection.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CU Boulder - Data Science\Spring 2024\Data Mining\Data_Backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f943686c21a634a0/Desktop/Data Mining/CSCI-Final-Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8632A504-ECB9-41F3-83C2-D8FB0D9BADB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{8632A504-ECB9-41F3-83C2-D8FB0D9BADB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6ECBEC7-1754-4487-B5A7-BC71436C19A6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EFA0F3B4-3249-4998-8A76-0DCAF9FCE7B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{EFA0F3B4-3249-4998-8A76-0DCAF9FCE7B8}"/>
   </bookViews>
   <sheets>
     <sheet name="productCollectionList" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="271">
   <si>
     <t>id</t>
   </si>
@@ -279,9 +279,6 @@
     <t>https://a.co/d/6pjCaNX</t>
   </si>
   <si>
-    <t>Iphone 14</t>
-  </si>
-  <si>
     <t>amazon2</t>
   </si>
   <si>
@@ -505,24 +502,6 @@
   </si>
   <si>
     <t>https://www.target.com/p/dyson-ball-animal-3-extra-upright-vacuum/-/A-85269264</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Hogwarts-Legacy-Xbox-English-Version-Region/dp/B0B9YSJC5S/ref=sr_1_2?crid=1K69XYMHWNR56&amp;dib=eyJ2IjoiMSJ9.Kg0XV9Kot63z1u2KagkEvpCVUtkbGXvapqAJX7afkiu3BdvCRxuMMxHq3-R-Vq88oqItB-jjTuSzsA4OUT3gHqxnGxm_W3ax9Bt1-kNDhIIrfk2DMuaREs1iW3ZpC41UpXGGXpnKaQWx_QR6PweYu_E0fgQaz6JOeKQrHgmpoGnZNkaPqUf-EzAWuLvi4LuOAF_AT5tsuZUIeboaBcrdGFpzu4TWaNBwkw4WmSvH7Vo.uFmuTgI86APUwJ8qSsprJqvZ4Dnr_EwLXhTo2K61-P0&amp;dib_tag=se&amp;keywords=hogwarts+legacy+xbox&amp;qid=1710278855&amp;sprefix=hogwarts+legacy+xbox%2Caps%2C129&amp;sr=8-2</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Star-Wars-Jedi-Survivor-Playstation-5/dp/B0BPD4JMWT/ref=sr_1_1?crid=1YEWINBQP33M2&amp;dib=eyJ2IjoiMSJ9.xmgn1bEBQh8fF6vN-_ijDTx3NnKfAvuz4KzU8chGgsL67cKZ-GVbOSb0nGWeW8mxQpNntErtqMVDRP2_Qvv6NVonWyAdXrQOG1vF3pQuiK5vfmslLzeTXkEtyMSwY0hE5dvkCY4Udzheb9VLdQgjV4RNjelCbXWMWS3HDuqkxw8RhbOBcyBB1KuJpYwpU0LO3JbTFOrTQoCecarfSPAyc01kEOKHqvHzXAHZPHjTRpo.vqAgJHJ_EuyQ0aHKHSEiLA9mvUUFdQtDGBvQua34gew&amp;dib_tag=se&amp;keywords=jedi+survivor+ps5&amp;qid=1710278950&amp;sprefix=jedi+survivor+ps%2Caps%2C174&amp;sr=8-1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Mario-Kart-8-Deluxe-Nintendo-Switch/dp/B01N1037CV/ref=sr_1_1?crid=1PYFQU1N4B68F&amp;dib=eyJ2IjoiMSJ9.8TZU_Of0o7Vk3YWNjDE9oY9I_W3GMrGxHT454fa05jnyQhIJ1QoKGzaub95DXly85ZIxHf3U7vByBD9UHUHObxJwp-_uYmPTubto19uqmmQglLhYd3W-DOvMZz4lfv1l9ezRsNuuryHtJljvddmeIZdaJWrxpna-VU5FHp3braflTwk_ypjvU7neyKr_vIay2KHtiMOKVjqNxAnzmGjWABX-bq-mvp-ghJ0Hq7eY9h4.vohI6h3tcX_pnwUMLahacLD3yr74bAsNKv9eeH5rAp0&amp;dib_tag=se&amp;keywords=mario+kart+8+deluxe&amp;qid=1710279189&amp;sprefix=mario+kart+%2Caps%2C167&amp;sr=8-1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Ninja-Woodfire-Technology-terracotta-OO101/dp/B0C6BQVDX3/ref=sr_1_3?crid=3DXGBNWLVTJHJ&amp;dib=eyJ2IjoiMSJ9.0WxsIb1exp9JW6Y3VWlsjnd4AbzdLgvTZ3dzGlCYh7z1OEIvxums8Mey72f26ju-BWrkrofq9sMNvCk49njaQbu-SN8ItGFSBFcq-t91Hsb6AE3rPWtoewiMwvt1h2JtkHhsZTKkYeLo0Y9nnD_eJ4STJOza34YIVUe9YB7S8nTqDnhXuTlMQ4TE6pHn3CnUHoVNJGIlgiU2ncUCADPEKpW5C2f1-rC8jpiw7k3qXsE.uqci_nwiB33tgkfGHQRjqPWrYYjoEoVkB-fSO930oYQ&amp;dib_tag=se&amp;keywords=Ninja%2BWoodfire%2BPizza%2BOven%2C%2B8-in-1%2BOutdoor%2BOven&amp;qid=1710280162&amp;sprefix=ninja%2Bwoodfire%2Bpizza%2Boven%2C%2B8-in-1%2Boutdoor%2Boven%2Caps%2C183&amp;sr=8-3&amp;th=1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/dp/B08YS7QZLL/ref=twister_B09V6MDSN6?_encoding=UTF8&amp;psc=1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Dyson-Animal-Extra-Upright-Vacuum/dp/B0B57QV5TT/ref=sr_1_3?crid=2IQWXZR08I144&amp;dib=eyJ2IjoiMSJ9.t3iEOoxEJUwLPVoSUcRptqioH5l2EvX8s4APBjqpAjI4e18xB7pmNY8TyLEanhvfvEQqqscP3Xi13oKWZQuQ1MaGTAAh82rbXWBT5nZjBYQqPFp7PUAvYcMk9RslrAyAZS0Nwv3r6RQ8M2iBSK7DQAZmAK0ycSydB1nB1cVDRVBJ0bgIwOtJPiE6ohrQceFbK44RLbkqiNcgSv_YM7QC30n8grFBmSgixz1fAwZtEd8.ZIHRSLxkS_22b7rx1F4ymcSJXsCEuBy_aVi0A1DzCpU&amp;dib_tag=se&amp;keywords=Dyson%2B-%2BBall%2BAnimal%2B3%2BExtra%2BUpright&amp;qid=1710280601&amp;sprefix=dyson%2B-%2Bball%2Banimal%2B3%2Bextra%2Bupright%2Caps%2C176&amp;sr=8-3&amp;th=1</t>
   </si>
   <si>
     <t>https://www.bestbuy.com/site/hogwarts-legacy-standard-edition-xbox-series-x/6502627.p?skuId=6502627</t>
@@ -739,6 +718,468 @@
     <t>Screen Size 6.1 inches
 Front-Facing Camera 12 megapixels
 Rear-Facing Camera 12 megapixels</t>
+  </si>
+  <si>
+    <t>Apple iPhone 14, 256GB, Blue - Unlocked (Renewed Premium)</t>
+  </si>
+  <si>
+    <t>Vibrant 6.1-inch Super Retina XDR display with OLED technology. Action mode for smooth, steady, handheld videos.
+High resolution and color accuracy make everything look sharp and true to life.
+New Main camera and improved image processing to capture your shots in all kinds of light - especially low light.
+4K Cinematic mode at 24 fps automatically shifts focus to the most important subject in a scene.
+A15 Bionic, with a 5‑core GPU for lightning-fast performance. Superfast 5G.</t>
+  </si>
+  <si>
+    <t>Brand - Apple
+Model Name - iPhone 14
+Wireless Carrier	 - Unlocked
+Operating System - iOS 15
+Cellular Technology - 5G
+Memory Storage Capacity - 256 GB
+Connectivity Technology	 - Wi-Fi
+Color - Blue
+Screen Size - 6.1 Inches
+Wireless network technology - GSM, LTE</t>
+  </si>
+  <si>
+    <t>Renewed Samsung Galaxy S22 Ultra 512GB - 8K Camera, S Pen, Long Battery, Fast Processor, Phantom Black</t>
+  </si>
+  <si>
+    <t>6.8", 1440 x 3088pixels, Infinity-O FHD+ Dynamic AMOLED 2X Display, 5000mAh Battery, Wireless Powershare
+512GB ROM, 12GB RAM, No SD Card Slot, Qualcomm SM8450 Snapdragon 8 Gen 1 (4nm), Octa-Core, Adreno 730
+Rear Camera: 108MP, f/1.8 + 10MP, f/4.9 + 10MP, f/2.4 + 12MP, f/2.2, Front Camera: 40MP, f/2.2, Android 12, One UI 4.1
+2G: GSM 850/900/1800/1900, CDMA 800/1900, 3G: HSDPA 850/900/1700(AWS)/1900/2100, CDMA2000 1xEV-DO, 4G LTE: 1/2/3/4/5/7/8/12/13/14/18/19/20/25/26/28/29/30/38/39/40/41/46/48/66/71, 5G: 1/3/5/7/8/20/28/38/41/66/71/260/261SA/NSA/Sub6/mmWave - Single SIM
+No Warranty. Compatible with Most GSM and CDMA Carriers like T-Mobile, AT&amp;T, MetroPCS, etc. Will Also work with CDMA Carriers Such as Verizon, Sprint.</t>
+  </si>
+  <si>
+    <t>Brand - SAMSUNG
+Model Name - Galaxy S22 Ultra 5G
+Wireless Carrier - Unlocked for All Carriers
+Operating System - Android
+Cellular Technology - 5G
+Memory Storage Capacity - 512 GB
+Connectivity Technology - Wi-Fi
+Color - Phantom Black
+Screen Size - 6.8 Inches
+Wireless network technology - Wi-Fi</t>
+  </si>
+  <si>
+    <t>HP DeskJet 2755e Wireless Color inkjet-printer, Print, scan, copy, Easy setup, Mobile printing, Best-for home, Instant Ink with HP+,white</t>
+  </si>
+  <si>
+    <t>PERFECT FOR HOME – Best for printing basic color documents like recipes, forms and travel documents. Print speeds up to 7.5 pages per minute in black or 5.5 pages per minute in color..Operating temperature range : 41 to 104°F / 5 to 40°C
+KEY FEATURES – Print, copy and scan in color, plus mobile and wireless printing
+INCLUDES FREE HP+ SMART FEATURES – Upgrade free to HP+ during setup to get advanced features for mobile printing, security, automatic updates and more. HP+ only works with an HP account, internet connection and Original HP Ink for the life of the printer.
+CONNECTIVITY – Dual-band Wi-Fi with self-reset automatically detects and resolves connectivity issues. Also includes USB 2.0 port.
+HP SMART APP – Simple, step-by-step guided setup. Print, scan, and copy everyday documents from your phone—from anywhere. Get advanced features with HP+ in the Smart app including mobile fax and advanced scanning features such as multi-item recognition.
+3 MONTHS OF INSTANT INK INCLUDED WITH HP+ – Print up to 700 pages a month and get ink delivered only when you need it. After 3 months, monthly fee applies unless cancelled, and you'll save up to 50% on ink.
+This printer is intended to work only with cartridges with original HP chips or circuitry and will block cartridges using non-HP chips or circuitry. Periodic firmware updates will maintain the effectiveness of these measures. Operating humidity range 20 to 80% RH (non-condensing).
+Dynamic security enabled printerCertain HP printers are intended to work only with cartridges that have a new or reused HP chip or electronic circuitry. These printers use dynamic security measures to block cartridges using a non-HP chip or electronic circuitry. Periodic firmware updates will maintain the effectiveness of these measures and block cartridges that previously worked. Reused HP chips and electronic circuitry enable the use of reused, re manufactured, and refilled cartridges.</t>
+  </si>
+  <si>
+    <t>Brand - HP
+Connectivity Technology - Wireless, USB
+Printing Technology - Inkjet
+Special Feature - auto-document feeder
+Color - white
+Model Name - 2755e
+Printer Output - Color
+Maximum Print Speed (Color) - 5.5 ppm
+Max Printspeed Monochrome - 7.5 ppm
+Item Weight - 7.55 Pounds</t>
+  </si>
+  <si>
+    <t>JBL Flip 5: Portable Wireless Bluetooth Speaker, IPX7 Waterproof - Black - Boomph's Comprehensive Ultimate Performance Cloth Solution for Your On-the-Go Sound Experience</t>
+  </si>
+  <si>
+    <t>Up to 20W of Audio Power | Bluetooth 4.2 Technology
+Supports A2DP, AVRCP | Plays up to 12 Hours on Full Charge
+IPX7 Waterproof Rating | PartyBoost Feature
+Tough and Durable | Made From 90% Recycled Plastic
+*PLEASE NOTE* - THE JBL FLIP 5 DOES *NOT* INCLUDE A USB WALL ADAPTER AND DOES *NOT* HAVE A 3.5mm AUX INPUT!</t>
+  </si>
+  <si>
+    <t>Brand - JBL
+Model Name - JBL Flip 5
+Speaker Type - Portable Bluetooth Speaker
+Connectivity Technology - Bluetooth
+Special Feature - waterproof, Stereo pairing</t>
+  </si>
+  <si>
+    <t>Microsoft 365 Family | 12-Month Subscription, Up to 6 People | Word, Excel, PowerPoint | 1TB OneDrive Cloud Storage | PC/MAC Instant Download | Activation Required</t>
+  </si>
+  <si>
+    <t>With 12 months of Microsoft 365 for up to six people, you and your family can have the tools to create, organize, and get things done.
+Bring out your best with premium Office apps, including Word, Excel, and PowerPoint.
+Your subscription includes 1 TB of OneDrive cloud storage for each person you share with, so they can easily access, edit, and share files and photos across all devices.
+Keep it all together with Outlook, an ad‑free app for your email, calendars, to do lists and contacts with security tools that keep your information protected.
+Protect your files with advanced security features like built‑in ransomware detection and recovery and you can use two‑step identity verification to access your most important files in OneDrive Personal Vault.
+Gives you the flexibility to use multiple PCs, Macs, iPads, iPhones and Android phones.</t>
+  </si>
+  <si>
+    <t>Platform: Subscription (PC/Mac)
+Edition: Microsoft 365 Family
+Subscription Term Name: Subscription - 12months</t>
+  </si>
+  <si>
+    <t>TurboTax Basic 2023 Tax Software, Federal Tax Return [PC/Mac Download]</t>
+  </si>
+  <si>
+    <t>Recommended for less-complex tax situations, claiming the Earned Income Tax Credit, or only need to file a Federal Tax Return.
+Includes 5 Federal e-files. State download and e-file additional. Free U.S.-based product support (hours may vary).
+Answer easy questions about your year and the right tax forms are filled in for you.
+TurboTax coaches you and double checks your return as you go.
+Up-to-date with the latest tax laws.</t>
+  </si>
+  <si>
+    <t>Platform For Display: Download
+Edition: Basic</t>
+  </si>
+  <si>
+    <t>Hamilton Beach 24782 Retro Toaster with Wide Slots, Sure-Toast echnology, Bagel &amp; Defrost Settings, Auto Boost to Lift Smaller Breads, 4 Slice, Polished Stainless Steel</t>
+  </si>
+  <si>
+    <t>EVENLY TOASTS BOTH SIDES OF SINGLE SLICE: With the Sure-Toast One Slice toast feature on the 4 slice toaster, you get perfectly toasted bread, with balanced color and texture on both sides every time you toast. Just press the One Slice button.
+EASILY RETRIEVE SMALLER BREADS: A convenient feature you won't find on all bread toasters, Auto Boost automatically lifts smaller breads like English muffins and gluten-free bread slices so they're easier to retrieve after toasting.
+FOOD THAT LOOKS AS GOOD AS IT TASTES: Even toasting improves color and texture of toast, English muffin, and sandwiches made with toasted breads.
+PERFECTLY TOASTS BAGELS: The bagel function toasts the cut side of the bagel and warms the outside for a great bagel-eating experience. You get crunchy, toasted bread on one side and warm, soft bread on the other.
+GIVE FROZEN FOODS EXTRA TIME TO COOK: Use the defrost setting for optimal cook time and flavor when toasting frozen breads and waffles. Just press one button to defrosts and toast.</t>
+  </si>
+  <si>
+    <t>Style: Toaster
+Brand - Hamilton Beach
+Color - Polished Stainless Steel
+Material - Stainless Steel
+Product Dimensions - 8.46"D x 11.81"W x 12.4"H
+Specific Uses For Product - Bagel</t>
+  </si>
+  <si>
+    <t>Razor MX350 Dirt Rocket Electric Motocross Off-Road Bike for Age 13+, Up to 30 Minutes Continuous Ride Time, 12" Air-Filled Tires, Hand-Operated Rear Brake, Twist Grip Throttle, Chain-Driven Motor</t>
+  </si>
+  <si>
+    <t>Authentic Motocross Frame Geometry, The Mx350 Scales Down The Dirt Bike To Size For Riders Ages 13+ And Up To 140 Lb (64 Kg).Fork: Double-crown, Grips: Soft, rubber..Cartoon character : Razor Motorcross
+High-Torque, Rear-Wheel Chain-Drive Delivers Increased Power And Traction
+Powers Riders At Speeds Of Up To 14 Mph (22 Km/H) With Up To 30 Minutes Of Continuous Use
+Features Adjustable-Angle, Riser-Style Handlebars, Spoked Wheels With 12" Pneumatic, Knobby Tires, Retractable Kickstand, And Hand-Operated Rear Brake
+24V (Two 12V) Sealed Lead-Acid Rechargeable Battery System</t>
+  </si>
+  <si>
+    <t>Max Rider Weight - 140 lbs (63 kg)
+Max Speed - 14 MPH (22.5 KPH)
+Battery - 24V, lead-acid
+Motor - 250W, single speed
+Run Time - Up to 30 mins
+Range - 7 miles (11 km)
+Brake - Hand operated, rear
+Wheels - 12" pneumatic
+Weight	 - 48.92 lbs (22.1 kg)</t>
+  </si>
+  <si>
+    <t>LG C3 Series 65-Inch Class OLED evo 4K Processor Smart Flat Screen TV for Gaming with Magic Remote AI-Powered OLED65C3PUA, 2023 with Alexa Built-in</t>
+  </si>
+  <si>
+    <t>LG OLED EVO: The LG OLED evo is powered by the a9 AI Processor Gen6—made exclusively for LG OLED—for beautiful picture and performance. The Brightness Booster improves brightness so you get luminous picture and high contrast, even in well-lit rooms.* AI-assisted deep learning analyzes what you're watching to choose the best picture and sound setting for your content.
+ULTRA SLIM DESIGN: The LG OLED evo C3 blends into the background with an almost invisible bezel for a seamless look. When you're finished watching, display paintings, photos and other content to blend the LG OLED evo C3 into your space.
+webOS 23 &amp; LG CHANNELS: Less searching, more streaming, thanks to the next generation of AI technology. Enjoy your favorite content including fitness, sports, entertainment and more. With Quick Cards, group your favorite apps into categories and use the Magic Remote to easily find what you're looking for. Get instant access to over 300 free channels with LG Channels.*
+DOLBY VISION + HOME THEATER: Experience the magic of the big screen right from your couch. Every LG OLED comes loaded with Dolby Vision for extraordinary color, contrast and brightness, plus Dolby Atmos* for wrap-around sound. Land in the center of the action with LG's FILMMAKER MODE, allowing you to see films just as the director intended.
+ULTIMATE GAMING: Packed with gaming features, the LG OLED evo C-Series comes with everything you need to win. Experience crisp, smooth imagery from a 0.1ms response time and native 120Hz refresh rate. All LG OLED TVs have NVIDIA G-Sync, AMD FreeSync Premium and VRR to further improve gaming quality. Four HDMI 2.1 inputs allow you to plug in all the devices you need. Whether you game on consoles or on the cloud,* the LG Game Dashboard and Game Optimizer put all the control at your fingertips.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Screen Size	65 Inches
+Brand	LG
+Supported Internet Services	Netflix, HBO Max, Disney Plus, Prime Video, Apple TV, Hulu, Paramount Plus, Peacock, Youtube TV, Spotify, iHeartRadio and more.Netflix, HBO Max, Disney Plus, Prime Video, Apple TV, Hulu, Paramount Plus, Peacock, Youtube TV, Spotify, iHeartR… See more
+Display Technology	OLED
+Product Dimensions	9.1"D x 56.7"W x 34.6"H
+Resolution	4K
+Refresh Rate	120
+Special Feature	AI Picture, AI Upscaling, FILMMAKER MODE, Picture Processor, Dolby Vision, Dynamic Tone Mapping, Dimming Technology, HDR (High Dynamic Range)AI Picture, AI Upscaling, FILMMAKER MODE, Picture Processor, Dolby Vision, Dynamic Tone Mapping, Dimming Tec… See more
+Model Name	C3
+Included Components	Remote Control Battery (AA x 2EA), Power Cable, Magic Remote, Quick Start Guide</t>
+  </si>
+  <si>
+    <t>GE APPLIANCES JES1460DSBB Countertop Microwave, 1.4 cu. ft, black</t>
+  </si>
+  <si>
+    <t>1.4 cu. ft. capacity
+Sensor cooking controls; Automatically adjusts time and power for delicious cooking results.
+Weight and time defrost: Simply enter the weight of the food, and the oven automatically sets the optimal defrosting time and power level or set your desired time for defrosting.
+Turntable: Rotates food throughout the cycle.
+Instant On controls: One-touch instant operation.</t>
+  </si>
+  <si>
+    <t>Brand	GE
+Product Dimensions	16.37"D x 21.87"W x 12.5"H
+Color	Black
+Capacity	1.4 Cubic Feet
+Special Feature	Express Cook - Instant-On 1-6, Shortcut Keys, Timer, Defrost, Turntable
+Recommended Uses For Product	Residential
+Installation Type	Countertop
+Wattage	1100 watts
+Material	Metal
+Included Components	Turntable</t>
+  </si>
+  <si>
+    <t>Windex Glass and Window Cleaner Spray Bottle, New Packaging Designed to Prevent Leakage and Breaking, Original Blue, 23 fl oz</t>
+  </si>
+  <si>
+    <t>Committed to bottles made from 100% recovered coastal plastic*
+*Recovered Coastal Plastic, in partnership with Plastic Bank, is post-consumer recycled plastic collected on land within 31 miles of an ocean so that it does not reach oceans or landfills.
+Windex Glass Cleaner leaves an unbeatable streak-free shine**
+**Based on Windex Original lab testing against leading competitor glass cleaners per Nielsen Scantrack US 52 weeks ended 3/29/19.
+Starts working on smudges and fingerprints even before you wipe</t>
+  </si>
+  <si>
+    <t>Size: 23 Fl Oz (Pack of 1)
+Brand	Windex
+Item Form	Liquid
+Scent	Original
+Specific Uses For Product	Window
+Material Feature	Recycled</t>
+  </si>
+  <si>
+    <t>Doritos, Nacho Cheese Flavored Tortilla Chips Party Size, 15 oz</t>
+  </si>
+  <si>
+    <t>Crest Cavity &amp; Tartar Protection Toothpaste, Whitening Baking Soda &amp; Peroxide, 5.7 oz, Pack of 2</t>
+  </si>
+  <si>
+    <t>Includes two 5.7 oz tubes of Crest Cavity &amp; Tartar Protection Toothpaste, Whitening Baking Soda &amp; Peroxide
+Contains baking soda and peroxide for a clean mounth feeling
+Whitens teeth by removing surface stains
+Gentle on tooth enamel
+Freshens breath for a clean feeling mouth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Brand	Crest
+Flavor	Mint
+Age Range (Description)	Adult
+Item Form	Paste
+Target Audience	Unisex Adults</t>
+  </si>
+  <si>
+    <t>OXO Good Grips 3-PC Small Square Short POP Container Set, White,Grey</t>
+  </si>
+  <si>
+    <t>The OXO good grips 3-piece POP container value set is airtight, stackable, space-efficient and now dishwasher safe, making it easy to keep your dry foods fresh and your countertops (and cabinets) clutter free
+Set includes: Three 1.1 Qt Containers ideal for 1 lb of brown or confectioner’s sugar, tea and snacks
+Push the button to engage the airtight seal. The button doubles as a handle for the lid
+Convenient fill line makes storing a cinch
+For best results, always use the button to open and close. Do not carry POP Containers by the lid
+BPA free. Top-rack dishwasher safe</t>
+  </si>
+  <si>
+    <t>Pattern Name: Set
+Brand	OXO
+Color	White, Grey, Clear
+Material	Plastic
+Material Feature	BPA Free
+Capacity	1 Liters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://a.co/d/igwagkv </t>
+  </si>
+  <si>
+    <t>Hogwarts Legacy - Xbox One | English | EU Version Region Free</t>
+  </si>
+  <si>
+    <t>EXPLORE AN OPEN WORLD. The wizarding world awaits you. Freely roam Hogwarts, Hogsmeade, the Forbidden Forest, and the surrounding Overland area.
+BE THE WITCH OR WIZARD YOU WANT TO BE. Learn spells, brew potions, grow plants, and tend to magical beasts along your journey. Get sorted into your house, forge relationships, and master skills to become the witch or wizard you want to be.
+EXPERIENCE A NEW WIZARDING WORLD ADVENTURE. Experience the wizarding world in an unexplored era to uncover a hidden truth from its past. Battle against trolls, Dark Wizards, goblins, and more as you face a dangerous villain threatening the fate of the wizarding world.
+Import Region Free PEGI Version</t>
+  </si>
+  <si>
+    <t>Product Dimensions	3.94 x 1.97 x 0.5 inches; 2.4 ounces
+Type of item	CD-ROM
+Language	English
+Item model number	5051892238106
+Item Weight	2.4 ounces
+Manufacturer	Warner Bros Interactive Entertainment UK
+Date First Available	January 8, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://a.co/d/g23bqY9 </t>
+  </si>
+  <si>
+    <t>Star Wars Jedi: Survivor - For Playstation 5</t>
+  </si>
+  <si>
+    <t>Continue Cal’s Journey – No longer a Padawan, Cal has come into his own and grown into a powerful Jedi Knight. Carrying the memories and expectations of the Jedi Order with him, his crusade against the Empire has only become more perilous
+Go Beyond Your Training – The cinematic combat system returns with additional Force abilities and new lightsaber fighting styles
+Explore an Untamed Galaxy – Discover new planets and familiar frontiers in the Star Wars galaxy, each with unique biomes, challenges, and enemies
+Master new skills, equipment, and abilities that will augment the ways you explore, fight, and roam</t>
+  </si>
+  <si>
+    <t>Package Dimensions	6.73 x 5.31 x 0.55 inches; 3.46 ounces
+Type of item	CD-ROM
+Item Weight	3.46 ounces
+Manufacturer	PlayStation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://a.co/d/i7CsVgM </t>
+  </si>
+  <si>
+    <t>Mario Kart 8 Deluxe - US Version</t>
+  </si>
+  <si>
+    <t>Hit the road with the definitive version of Mario Kart 8 and play anytime, anywhere. Race your friends or battle them in a revised battle mode for new and returning battle courses
+Play locally in up to 4-player multiplayer in 1080p while playing in TV Mode. Every track of the Wii U version, including DLC, makes a glorious return
+Plus, the Inklings appear at all-new guest characters, along with returning favorites, such as King Boo, Dry Bones, and Bowser Jr.
+Players can choose a new Smart Steering feature which makes driving and staying on the track easy for novice players and kids even at 200cc</t>
+  </si>
+  <si>
+    <t>Platform For Display: Nintendo Switch
+Edition: Standard
+Type of item	Video Game
+Language	English
+Item Weight	2.08 ounces
+Manufacturer	Nintendo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://a.co/d/0WIFDVd </t>
+  </si>
+  <si>
+    <t>Ninja Woodfire Pizza Oven, 8-in-1 outdoor oven, 5 Pizza Settings, Ninja Woodfire Technology, 700°F high heat, BBQ smoker, wood pellets, pizza stone, electric heat, portable, terracotta red, 9x13</t>
+  </si>
+  <si>
+    <t>8-IN-1 FUNCTIONALITY: Do more outdoors and turn any space into an outdoor kitchen; Pizza, Max Roast, Specialty Roast, Broil, Bake, Smoker, Dehydrate and Keep Warm.
+ARTISAN PIZZAS: 3-minute no turn, no fuss pizzas. Choose from 5 different settings to satisfy any craving; Neapolitan, Thin Crust, Pan, New York, and Frozen. *cooked at 700°F excludes 25-minute preheat.
+700°F PREMIUM RESULTS: Brick oven-inspired results without the hassle—charring, caramelization, blistering and crunch for premium textures and flavors.
+FEED A CROWD: Fit up to 12-lb turkey, 9-lb pork shoulder, 12-lb prime rib dinner with veggies, 12-inch pizza, full sheet-pan meal or a standard 8x11 casserole dish.
+SMOKY FLAVORS ON ANYTHING: Add authentic BBQ flavors to anything you make with just 1/2 cup of pellets at any temperature up to 700°F.
+COMPLETE TEMPERATURE CONTROL: No flame, full control. Electric heat unlocks a wide range of temps from 105-700°F. Expand your horizons and cook more outdoors.
+HIGH HEAT ROASTER: 700°F max heat for Max Roast and Specialty Roast. Get high-heat char on steaks in under 7 mins, full meals up to 40% faster*, or cook a full roast with crispy outsides and juicy insides. *vs. indoor oven. Excludes 25-minute preheat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Brand	Ninja
+Color	Terracotta Red
+Product Dimensions	21.5"D x 18"W x 15.1"H
+Special Feature	Auto Cook, Timer, Racks, Programmable
+Control Type	Knob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://a.co/d/4IvJv28 </t>
+  </si>
+  <si>
+    <t>Igloo 24 qt IMX Lockable Insulated Ice Chest Injection Molded Cooler</t>
+  </si>
+  <si>
+    <t>Ultratherm insulation in the body &amp; lid provides four days of ice retention
+Holds up to 35 cans
+Cool Riser Technology improves cooling performance
+Removable wire basket
+Anti-skid feet on the base keep the cooler stable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Brand	Igloo
+Color	Gray
+Material	Plastic
+Package Information	Bottle,Cans,Cup
+Capacity	24 Quarts
+Item Weight	16.45 Pounds
+Special Feature	Lightweight
+Included Components	Bottle opener
+Recommended Uses For Product	Camping
+Model Name	IMX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://a.co/d/88HEXAh </t>
+  </si>
+  <si>
+    <t>The best cleaning performance of any upright de-tangling vacuum.¹
+Engineered for larger homes with pets. Removes dirt and pet hair around your home. Easily tackles big messes. With two additional specialized pet tools.
+De-tangling technology. Automatically clears wrapped hair from the brush bar as you clean.
+Specialized pet tools. Pet groom tool for medium and long-haired pets.² Tangle-free turbine tool removes pet hair from upholstery and cars.
+Ball technology. Navigate around obstacles with a simple turn of the wrist. For easy, precise maneuvering around your home.
+3 cleaning modes. Select the right cleaning mode for the right task. Optimized for a variety of floor types, for complete control over your clean.
+5 Dyson-engineered accessories. Tangle-free turbine tool, Pet groom tool, tool holder, stair tool, combination toolThe best cleaning performance of any upright de-tangling vacuum.¹
+Engineered for larger homes with pets. Removes dirt and pet hair around your home. Easily tackles big messes. With two additional specialized pet tools.
+De-tangling technology. Automatically clears wrapped hair from the brush bar as you clean.
+Specialized pet tools. Pet groom tool for medium and long-haired pets.² Tangle-free turbine tool removes pet hair from upholstery and cars.
+Ball technology. Navigate around obstacles with a simple turn of the wrist. For easy, precise maneuvering around your home.
+3 cleaning modes. Select the right cleaning mode for the right task. Optimized for a variety of floor types, for complete control over your clean.
+5 Dyson-engineered accessories. Tangle-free turbine tool, Pet groom tool, tool holder, stair tool, combination tool</t>
+  </si>
+  <si>
+    <t>Brand	Dyson
+Special Feature	De-tangling Motorbar™ cleaner head, Corded, Whole-machine filtration, Pet groom tool, Bagless
+Filter Type	Washable
+Included Components	Tangle-free turbine tool, Combination Tool, Stair tool, Dyson Ball Animal 3 Extra upright vacuum cleaner, Pet groom tool, Tool holderTangle-free turbine tool, Combination Tool, Stair tool, Dyson Ball Animal 3 Extra upright vacuum cleaner, Pet groom tool, Tool holder</t>
+  </si>
+  <si>
+    <t>RICHLY PIGMENTED, BOLD LIPSTICK: Serve up your best O face with bold, satiny color in one single swipe that creates a satin finish.
+HYDRATING &amp; LONG-LASTING FORMULA: e.l.f. Cosmetics’ O Face Satin Lipstick's creamy, long-lasting formula is infused with nourishing &amp; hydrating squalane and jojoba esters for a super-comfortable, next-to-nothing feel.
+AVAILABLE IN 20 SHADES: e.l.f. O Face Satin Lipstick is available in 20 sultry shades. Dirty Talk is a beige pink.
+BEAUTY TIP: Exfoliate lips with e.l.f.’s Lip Exfoliator, use our e.l.f. Love Triangle Lip Filler Liner to line, and finish with the O Face Satin Lipstick for a complete lip look. Dirty Talk goes great with Love Triangle Lip Filler Liner in Soft Pink.
+SKIN-LOVING INGREDIENTS: All e.l.f. products are made from skin-loving ingredients you want, minus the toxins you don’t—all at good-for-you prices. All e.l.f. products are 100% cruelty-free and Vegan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Brand	e.l.f.
+Color	No Regrets
+Skin Type	All
+Item Form	Pencil
+Finish Type	Satin</t>
+  </si>
+  <si>
+    <t>SKIN-CARING: Radiance is boosted, the appearance of fine lines and wrinkles is reduced in 4 weeks, and skin elasticity is improved over time
+BENEFITS: Skin-caring foundation leaves skin looking healthy, plump, and naturally radiant
+INGREDIENTS: Infused with 5% Squalane + Hyaluronic acid
+COVERAGE: Medium coverage
+FIND YOUR SHADE: 28 buildable shades</t>
+  </si>
+  <si>
+    <t>Item Form	Cream
+Color	Creamy Natural
+Skin Type	All
+Finish Type	Radiant
+Recommended Uses For Product	Face Makeup</t>
+  </si>
+  <si>
+    <t>LEYAOYAO Cube Bookshelf 3 Tier Mid-Century Rustic Brown Modern Bookcase with Legs</t>
+  </si>
+  <si>
+    <t>【Vibrant Mid-Century Modern Bookshelf】 The 3 tier bookshelf is brought to life by a special mysterious brown and crisscross partition design. The unique appearance allows you to enjoy both retro and modern styles. Reshape your storage space with LEYAOYAO’s charming vintage brown modern cube bookshelves, making your home/office/school more elegant and stylish.
+【Reliable Materials &amp; Sturdy Structure】This durable 3 shelf bookcase is made of high quality board with high glossy finish veneer. Single weight capacity of each open cube shelf is up to 35 lbs. The canted legs of this standing bookcase are environmentally friendly thick plastic supported by four metal screws for extra stability.
+【Suitable Size &amp; Great Display】The simple upright and open design of the book shelves can help you to save much more space in your house. This brown bookshelf can be used as a storage shelf organizer and display shelf rack. Fill this creative display cabinet with your favorites! Choose a best display organizer for your books, CDs, magazines, and collections! Product size:31.5"L x 9.45" W x 43.31" H
+【Thicker Packaging &amp; Easy to Install】 We packaged the bookcases particularly with thickened foams and firmed edges to protect it in good condition upon arriving. The rustic wood bookshelf comes with step-by-step instructions, all numbered parts and extra tools for your convenience.
+【Considerate Details】All decorative wood cube storage organizer bookshelves come with full unit back pieces to prevent the shelf from wobbling or separating apart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Room Type	Office, Living Room, Bedroom
+Number of Shelves	7
+Special Feature	Sturdy
+Product Dimensions	9.45"D x 31.5"W x 43.3"H
+Style	Vintage_style
+Age Range (Description)	Adult
+Brand	LEYAOYAO
+Product Care Instructions	Wipe with Dry Cloth
+Size	7 Cube
+Weight Limit	35 Pounds</t>
+  </si>
+  <si>
+    <t>REVERSIBLE OTTOMAN: This sofa turns modular with an independent matching ottoman that can conveniently be placed on either side for a versatile chaise lounger design
+MULTIPURPOSE DESIGN: An attractive, multipurpose design makes it perfect for various spaces such as your living room, college dorm, home office, and more
+QUALITY CONSTRUCTION: Crafted with super soft fabric and a sturdy wood frame, helping ensure a sofa that keeps you and guests comfortable for years to come
+ROOM FOR 3: Designed for compact areas such as an apartment or bonus room, with a space-saving yet heavy-duty design that allows for up to 3 people and 680 pounds
+EASY, TOOL FREE ASSEMBLY: Put it together in as little as 15 minutes by aligning brackets and screwing a few pieces together before opening up the seat and back cushions for comfy lounging; OVERALL DIMENSIONS (w/ Ottoman): 78"(L) x 54"(W) x 34"(H); WEIGHT CAPACITY: 680lbs.; Items contained in 2 separate boxes. Transportation times may vary per box.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Brand	Best Choice Products
+Assembly Required	Yes
+Seat Depth	24 inches
+Seat Height	18 Inches
+Weight Limit	680 Pounds
+Product Dimensions	52"D x 78"W x 34"H
+Item Weight	106 Pounds
+Leg Length	4 Inches
+Type	Sofa Chaise
+Color	Blue/Gray</t>
   </si>
 </sst>
 </file>
@@ -802,16 +1243,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -819,6 +1258,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1163,14 +1605,14 @@
       <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" customWidth="1"/>
+    <col min="4" max="4" width="47.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1182,30 +1624,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1216,32 +1658,32 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+    <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+    <row r="7" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1252,8 +1694,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1264,8 +1706,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1276,11 +1718,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="1"/>
@@ -1288,8 +1730,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+    <row r="11" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1300,8 +1742,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1310,8 +1752,8 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1322,8 +1764,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1334,89 +1776,89 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+    <row r="15" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B43" s="1" t="s">
         <v>32</v>
       </c>
@@ -1424,7 +1866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
         <v>33</v>
       </c>
@@ -1432,31 +1874,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B45" s="1"/>
       <c r="D45" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B46" s="1"/>
       <c r="D46" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B47" s="1"/>
       <c r="D47" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B48" s="1"/>
       <c r="D48" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B49" s="1" t="s">
         <v>38</v>
       </c>
@@ -1464,7 +1906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B50" s="1" t="s">
         <v>8</v>
       </c>
@@ -1472,19 +1914,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B51" s="1"/>
       <c r="D51" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B52" s="1"/>
       <c r="D52" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
         <v>40</v>
       </c>
@@ -1492,7 +1934,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B54" s="1" t="s">
         <v>41</v>
       </c>
@@ -1500,25 +1942,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B59" s="1"/>
       <c r="D59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B60" s="1" t="s">
         <v>43</v>
       </c>
@@ -1526,19 +1968,19 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B61" s="1"/>
       <c r="D61" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B62" s="1"/>
       <c r="D62" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B63" s="1" t="s">
         <v>45</v>
       </c>
@@ -1546,7 +1988,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B64" s="1" t="s">
         <v>47</v>
       </c>
@@ -1554,12 +1996,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B65" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B66" s="1" t="s">
         <v>49</v>
       </c>
@@ -1567,7 +2009,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B67" s="1" t="s">
         <v>51</v>
       </c>
@@ -1575,7 +2017,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B68" s="1" t="s">
         <v>52</v>
       </c>
@@ -1595,33 +2037,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8FFCC8-FB4D-413C-81EB-800110419A65}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" customWidth="1"/>
-    <col min="4" max="4" width="98.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="32.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.90625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33" style="1" customWidth="1"/>
+    <col min="7" max="8" width="66.81640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.81640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1639,875 +2081,1281 @@
       <c r="I1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>140</v>
+      <c r="D4" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>141</v>
+      <c r="D5" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>67</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+    <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C7" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>68</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+    <row r="8" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+    <row r="9" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>70</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="D10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="11" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>72</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+    <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>73</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="14" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>75</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="C16" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="C17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="C18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+    <row r="19" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="C19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+    <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="C20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="21" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="C21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C23" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C24" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C25" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C26" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C27" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C28" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C29" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="30" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
         <v>1</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I30" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="J30" s="1">
+        <v>101</v>
+      </c>
+      <c r="K30" s="1">
+        <v>664.71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="174" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>2</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="C31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I31" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="J31" s="1">
+        <v>356</v>
+      </c>
+      <c r="K31" s="1">
+        <v>619.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="406" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>3</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="D32" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="C32" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="F32" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="I32" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J32" s="1">
+        <v>8044</v>
+      </c>
+      <c r="K32" s="1">
+        <v>49.89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
         <v>4</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C33" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="F33" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="I33" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="J33" s="1">
+        <v>365</v>
+      </c>
+      <c r="K33" s="1">
+        <v>89.95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="203" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
         <v>5</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C34" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="F34" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I34" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J34" s="1">
+        <v>305</v>
+      </c>
+      <c r="K34" s="1">
+        <v>99.99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
         <v>6</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C35" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="F35" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I35" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="J35" s="1">
+        <v>46</v>
+      </c>
+      <c r="K35" s="1">
+        <v>39.99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
         <v>7</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="C36" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="F36" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I36" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="J36" s="1">
+        <v>78</v>
+      </c>
+      <c r="K36" s="1">
+        <v>49.98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
         <v>8</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C37" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="F37" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I37" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J37" s="1">
+        <v>2165</v>
+      </c>
+      <c r="K37" s="1">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
         <v>9</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="I38" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J38" s="1">
+        <v>322</v>
+      </c>
+      <c r="K38" s="1">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>10</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>10</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="D39" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C39" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="F39" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I39" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="J39" s="1">
+        <v>126</v>
+      </c>
+      <c r="K39" s="1">
+        <v>139.99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
         <v>11</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C40" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="F40" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I40" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="J40" s="1">
+        <v>204</v>
+      </c>
+      <c r="K40" s="1">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
         <v>12</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="C41" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="F41" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
         <v>13</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C42" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="F42" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I42" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="J42" s="1">
+        <v>9</v>
+      </c>
+      <c r="K42" s="1">
+        <v>6.29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
         <v>14</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C43" t="s">
-        <v>77</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="F43" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="I43" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J43" s="1">
+        <v>415</v>
+      </c>
+      <c r="K43" s="1">
+        <v>31.99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
         <v>15</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I44" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="J44" s="1">
+        <v>28</v>
+      </c>
+      <c r="K44" s="1">
+        <v>39.85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>16</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="D45" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I45" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J45" s="1">
         <v>16</v>
       </c>
-      <c r="B45" t="s">
+      <c r="K45" s="1">
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>17</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>17</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="D46" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I46" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J46" s="1">
+        <v>6453</v>
+      </c>
+      <c r="K46" s="1">
+        <v>39.99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>18</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>18</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="D47" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="I47" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J47" s="1">
+        <v>150</v>
+      </c>
+      <c r="K47" s="1">
+        <v>349.99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>19</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>19</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="D48" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="I48" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J48" s="1">
+        <v>122</v>
+      </c>
+      <c r="K48" s="1">
+        <v>94.99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="377" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>20</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>20</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="D49" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I49" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J49" s="1">
+        <v>357</v>
+      </c>
+      <c r="K49" s="1">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>21</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>21</v>
-      </c>
-      <c r="B50" t="s">
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>22</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>22</v>
-      </c>
-      <c r="B51" t="s">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>23</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>23</v>
-      </c>
-      <c r="B52" t="s">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>24</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>24</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
+        <v>25</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>25</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
+        <v>26</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>26</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="56" spans="1:11" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>27</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>27</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="D56" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C56" t="s">
-        <v>77</v>
-      </c>
-      <c r="D56" s="3" t="s">
+      <c r="E56" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="1" t="s">
-        <v>120</v>
+      <c r="G56" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>263</v>
       </c>
       <c r="I56" s="1">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J56" s="4">
-        <v>1603</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="J56" s="6">
+        <v>312</v>
+      </c>
+      <c r="K56" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
         <v>28</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C57" t="s">
-        <v>77</v>
-      </c>
-      <c r="D57" s="3" t="s">
+      <c r="E57" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="1" t="s">
-        <v>123</v>
+      <c r="G57" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>265</v>
       </c>
       <c r="I57" s="1">
         <v>4.2</v>
       </c>
-      <c r="J57" s="4">
-        <v>1488</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="J57" s="6">
+        <v>386</v>
+      </c>
+      <c r="K57" s="1">
+        <v>13.48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
         <v>29</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C58" t="s">
-        <v>77</v>
-      </c>
-      <c r="D58" s="3" t="s">
+      <c r="E58" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="1" t="s">
-        <v>126</v>
+      <c r="G58" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>268</v>
       </c>
       <c r="I58" s="1">
         <v>4.5</v>
       </c>
-      <c r="J58" s="4">
-        <v>1979</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A59">
+      <c r="J58" s="6">
+        <v>566</v>
+      </c>
+      <c r="K58" s="1">
+        <v>99.98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="232" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
         <v>30</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C59" t="s">
-        <v>77</v>
-      </c>
-      <c r="D59" s="3" t="s">
+      <c r="E59" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="1" t="s">
-        <v>129</v>
+      <c r="G59" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>270</v>
       </c>
       <c r="I59" s="1">
         <v>4</v>
       </c>
-      <c r="J59" s="4">
-        <v>1696</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="65" spans="3:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
-        <v>130</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>203</v>
+      <c r="J59" s="6">
+        <v>502</v>
+      </c>
+      <c r="K59" s="1">
+        <v>359.99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C60" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C61" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C62" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C63" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C64" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="3:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C65" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I65" s="1">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J65">
+      <c r="J65" s="1">
         <v>211</v>
       </c>
-      <c r="K65">
+      <c r="K65" s="1">
         <v>729.99</v>
       </c>
     </row>
-    <row r="66" spans="3:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
-        <v>130</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>200</v>
+    <row r="66" spans="3:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="C66" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="I66" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="J66">
+      <c r="J66" s="1">
         <v>396</v>
       </c>
-      <c r="K66">
+      <c r="K66" s="1">
         <v>1199.99</v>
       </c>
     </row>
-    <row r="67" spans="3:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
-        <v>130</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>197</v>
+    <row r="67" spans="3:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="C67" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="I67" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="J67">
+      <c r="J67" s="1">
         <v>3496</v>
       </c>
-      <c r="K67">
+      <c r="K67" s="1">
         <v>49.99</v>
       </c>
     </row>
-    <row r="68" spans="3:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
+    <row r="68" spans="3:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="C68" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="F68" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F68" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="H68" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="I68" s="1">
         <v>4.8</v>
       </c>
-      <c r="J68">
+      <c r="J68" s="1">
         <v>5938</v>
       </c>
-      <c r="K68">
+      <c r="K68" s="1">
         <v>89.99</v>
       </c>
     </row>
-    <row r="69" spans="3:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>130</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E69" s="1"/>
+    <row r="69" spans="3:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="C69" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>185</v>
+      </c>
       <c r="F69" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="I69" s="1">
         <v>4.5</v>
@@ -2515,23 +3363,23 @@
       <c r="J69" s="1">
         <v>10362</v>
       </c>
-      <c r="K69">
+      <c r="K69" s="1">
         <v>99.99</v>
       </c>
     </row>
-    <row r="70" spans="3:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>130</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="E70" s="3"/>
+    <row r="70" spans="3:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="C70" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E70" s="2"/>
       <c r="F70" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="I70" s="1">
         <v>4.5999999999999996</v>
@@ -2539,23 +3387,23 @@
       <c r="J70" s="1">
         <v>315</v>
       </c>
-      <c r="K70">
+      <c r="K70" s="1">
         <v>69.989999999999995</v>
       </c>
     </row>
-    <row r="71" spans="3:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
-        <v>130</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="E71" s="3"/>
+    <row r="71" spans="3:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="C71" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E71" s="2"/>
       <c r="F71" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="I71" s="1">
         <v>4.5</v>
@@ -2563,23 +3411,23 @@
       <c r="J71" s="1">
         <v>28</v>
       </c>
-      <c r="K71">
+      <c r="K71" s="1">
         <v>49.99</v>
       </c>
     </row>
-    <row r="72" spans="3:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
-        <v>130</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="E72" s="3"/>
+    <row r="72" spans="3:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="C72" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E72" s="2"/>
       <c r="F72" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="I72" s="1">
         <v>4.4000000000000004</v>
@@ -2587,20 +3435,20 @@
       <c r="J72" s="1">
         <v>200</v>
       </c>
-      <c r="K72">
+      <c r="K72" s="1">
         <v>339.99</v>
       </c>
     </row>
-    <row r="73" spans="3:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
-        <v>130</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="E73" s="3"/>
+    <row r="73" spans="3:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C73" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E73" s="2"/>
       <c r="F73" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="I73" s="1">
         <v>4.8</v>
@@ -2608,23 +3456,23 @@
       <c r="J73" s="1">
         <v>1499</v>
       </c>
-      <c r="K73">
+      <c r="K73" s="1">
         <v>1599.99</v>
       </c>
     </row>
-    <row r="74" spans="3:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
-        <v>130</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E74" s="3"/>
+    <row r="74" spans="3:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="C74" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E74" s="2"/>
       <c r="F74" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="I74" s="1">
         <v>4</v>
@@ -2632,22 +3480,22 @@
       <c r="J74" s="1">
         <v>860</v>
       </c>
-      <c r="K74">
+      <c r="K74" s="1">
         <v>139.99</v>
       </c>
     </row>
-    <row r="75" spans="3:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
-        <v>130</v>
-      </c>
-      <c r="D75" s="3" t="s">
+    <row r="75" spans="3:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="C75" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H75" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="I75" s="1">
         <v>4.8</v>
@@ -2655,22 +3503,22 @@
       <c r="J75" s="1">
         <v>380</v>
       </c>
-      <c r="K75">
+      <c r="K75" s="1">
         <v>44.99</v>
       </c>
     </row>
-    <row r="76" spans="3:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
-        <v>130</v>
-      </c>
-      <c r="D76" s="3" t="s">
+    <row r="76" spans="3:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="C76" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F76" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F76" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="H76" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I76" s="1">
         <v>4.7</v>
@@ -2678,22 +3526,22 @@
       <c r="J76" s="1">
         <v>1527</v>
       </c>
-      <c r="K76">
+      <c r="K76" s="1">
         <v>34.99</v>
       </c>
     </row>
-    <row r="77" spans="3:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>130</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>163</v>
+    <row r="77" spans="3:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="C77" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="I77" s="1">
         <v>4.9000000000000004</v>
@@ -2701,22 +3549,22 @@
       <c r="J77" s="1">
         <v>32562</v>
       </c>
-      <c r="K77">
+      <c r="K77" s="1">
         <v>39.99</v>
       </c>
     </row>
-    <row r="78" spans="3:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
-        <v>130</v>
-      </c>
-      <c r="D78" s="3" t="s">
+    <row r="78" spans="3:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="C78" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="H78" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="I78" s="1">
         <v>4.8</v>
@@ -2724,22 +3572,22 @@
       <c r="J78" s="1">
         <v>106</v>
       </c>
-      <c r="K78">
+      <c r="K78" s="1">
         <v>349.99</v>
       </c>
     </row>
-    <row r="79" spans="3:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
-        <v>130</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>164</v>
+    <row r="79" spans="3:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="C79" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="I79" s="1">
         <v>4.5999999999999996</v>
@@ -2747,22 +3595,22 @@
       <c r="J79" s="1">
         <v>41</v>
       </c>
-      <c r="K79">
+      <c r="K79" s="1">
         <v>94.99</v>
       </c>
     </row>
-    <row r="80" spans="3:11" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
-        <v>130</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>165</v>
+    <row r="80" spans="3:11" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="C80" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="I80" s="1">
         <v>4.5999999999999996</v>
@@ -2770,55 +3618,38 @@
       <c r="J80" s="1">
         <v>777</v>
       </c>
-      <c r="K80">
+      <c r="K80" s="1">
         <v>399.99</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D30" r:id="rId1" xr:uid="{130ED931-C0D5-4631-8A44-4F9CED526F3D}"/>
-    <hyperlink ref="D31" r:id="rId2" xr:uid="{A76F5837-6645-4380-8C05-A032935932AA}"/>
-    <hyperlink ref="D32" r:id="rId3" xr:uid="{F4B38194-9784-42C6-B5FB-5DC0352BF3BC}"/>
-    <hyperlink ref="D33" r:id="rId4" xr:uid="{8EB8E547-29B8-4034-BC7A-1E38C13302F7}"/>
-    <hyperlink ref="D34" r:id="rId5" xr:uid="{D3B90A15-B487-4718-B67A-D9A783549002}"/>
-    <hyperlink ref="D35" r:id="rId6" xr:uid="{9240A67F-E936-4A7A-B8DD-99B93704DFD3}"/>
-    <hyperlink ref="D36" r:id="rId7" xr:uid="{15A49671-BF18-4C6B-8525-B693F179BD7A}"/>
-    <hyperlink ref="D37" r:id="rId8" xr:uid="{6221B301-6B94-46CC-8728-319A961E1C22}"/>
-    <hyperlink ref="D38" r:id="rId9" xr:uid="{0EA6C536-7C11-4E3B-A72C-D044F33EDC31}"/>
-    <hyperlink ref="D39" r:id="rId10" xr:uid="{EE7EB3A1-A27F-4709-AEEC-F8067DA82420}"/>
-    <hyperlink ref="D40" r:id="rId11" xr:uid="{68263586-9729-4689-A0D1-406BD38D45D8}"/>
-    <hyperlink ref="D41" r:id="rId12" xr:uid="{CA9189C5-F2CE-48A8-AAF3-BBE8517CE44B}"/>
-    <hyperlink ref="D42" r:id="rId13" xr:uid="{C44812AC-BA35-4E7E-8174-CAE21A17EAAE}"/>
-    <hyperlink ref="D43" r:id="rId14" xr:uid="{6276CFCE-9952-42A8-BA0A-B30C727BE342}"/>
-    <hyperlink ref="D56" r:id="rId15" xr:uid="{911155BB-A88A-4C90-A863-325DCD0E385B}"/>
-    <hyperlink ref="D57" r:id="rId16" xr:uid="{445282CD-8591-4C05-BE45-9FDE0FC92D35}"/>
-    <hyperlink ref="D58" r:id="rId17" xr:uid="{FBBAEFD8-1EA7-4308-A8DB-5B363FDE6573}"/>
-    <hyperlink ref="D59" r:id="rId18" xr:uid="{0D5F9383-36E8-4E03-BE21-427ED2729086}"/>
-    <hyperlink ref="D2" r:id="rId19" xr:uid="{CAD9AB78-FE3F-45E3-A8C4-3091ADF185E8}"/>
-    <hyperlink ref="D3" r:id="rId20" xr:uid="{0590ADB1-8931-47E6-A9F9-635B5C713D11}"/>
-    <hyperlink ref="D6" r:id="rId21" xr:uid="{8E2BE472-0220-4AFC-8868-DD61E717ED8A}"/>
-    <hyperlink ref="D7" r:id="rId22" xr:uid="{A2F21B63-6932-487D-8998-597425811A48}"/>
-    <hyperlink ref="D8" r:id="rId23" xr:uid="{79C1DC41-5DBC-4BDB-BDF0-84E81FA68FA1}"/>
-    <hyperlink ref="D9" r:id="rId24" xr:uid="{1EBCD253-DB99-4828-A82C-95E26C544FCB}"/>
-    <hyperlink ref="D11" r:id="rId25" xr:uid="{DB4CBE25-561E-4694-B7E1-01D96706296F}"/>
-    <hyperlink ref="D14" r:id="rId26" xr:uid="{09675619-C1DA-4BC4-A080-53E08339B896}"/>
-    <hyperlink ref="D15" r:id="rId27" xr:uid="{1CD5ED3E-0215-488D-8CF9-29EE2B7F29F6}"/>
-    <hyperlink ref="D12" r:id="rId28" xr:uid="{F5BD0E9E-68D4-4B40-A9D0-59034348797F}"/>
-    <hyperlink ref="D13" r:id="rId29" xr:uid="{61558A01-8BE8-49DB-8FDF-7949BD05D0CA}"/>
-    <hyperlink ref="D4" r:id="rId30" xr:uid="{D38CDF7D-9FE1-49F1-A1F8-28032F04F6AB}"/>
-    <hyperlink ref="D5" r:id="rId31" xr:uid="{530D22AE-701B-4A32-9512-660098BBDF57}"/>
-    <hyperlink ref="D10" r:id="rId32" xr:uid="{A8923910-483F-46D2-8ED9-C10E6AF959E8}"/>
-    <hyperlink ref="D78" r:id="rId33" xr:uid="{DB2F31ED-A20B-4C8C-8687-199BB200EF6C}"/>
-    <hyperlink ref="D75" r:id="rId34" xr:uid="{7D001425-952B-4273-9E9A-FCE3CB5FFF9A}"/>
-    <hyperlink ref="D76" r:id="rId35" xr:uid="{156ECCF7-0BD4-43A9-B176-59C6D564886B}"/>
-    <hyperlink ref="D77" r:id="rId36" xr:uid="{918848D8-7BE5-4018-8C55-CEC7002CA9F2}"/>
-    <hyperlink ref="D79" r:id="rId37" xr:uid="{8E1E973E-3ACA-4E7C-AD67-B499DA21FEA1}"/>
-    <hyperlink ref="D80" r:id="rId38" xr:uid="{4FD46094-DAB9-4CD6-A190-C0C6227810FC}"/>
-    <hyperlink ref="D69" r:id="rId39" xr:uid="{7716567D-D933-48C2-9224-35CA8B300709}"/>
-    <hyperlink ref="D68" r:id="rId40" xr:uid="{6E2FCDC0-D3E2-4E28-9D42-F1F93D03797C}"/>
-    <hyperlink ref="D67" r:id="rId41" xr:uid="{417AACA0-6100-426E-85C1-0AF8CC02E529}"/>
-    <hyperlink ref="D66" r:id="rId42" xr:uid="{DAC37E6D-5373-4CEA-BF1C-8C46D88AC0DF}"/>
-    <hyperlink ref="D65" r:id="rId43" xr:uid="{1FD7B0EC-16E0-4C60-AE94-7B4720546328}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{CAD9AB78-FE3F-45E3-A8C4-3091ADF185E8}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{0590ADB1-8931-47E6-A9F9-635B5C713D11}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{8E2BE472-0220-4AFC-8868-DD61E717ED8A}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{A2F21B63-6932-487D-8998-597425811A48}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{79C1DC41-5DBC-4BDB-BDF0-84E81FA68FA1}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{1EBCD253-DB99-4828-A82C-95E26C544FCB}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{DB4CBE25-561E-4694-B7E1-01D96706296F}"/>
+    <hyperlink ref="D14" r:id="rId8" xr:uid="{09675619-C1DA-4BC4-A080-53E08339B896}"/>
+    <hyperlink ref="D15" r:id="rId9" xr:uid="{1CD5ED3E-0215-488D-8CF9-29EE2B7F29F6}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{F5BD0E9E-68D4-4B40-A9D0-59034348797F}"/>
+    <hyperlink ref="D13" r:id="rId11" xr:uid="{61558A01-8BE8-49DB-8FDF-7949BD05D0CA}"/>
+    <hyperlink ref="D4" r:id="rId12" xr:uid="{D38CDF7D-9FE1-49F1-A1F8-28032F04F6AB}"/>
+    <hyperlink ref="D5" r:id="rId13" xr:uid="{530D22AE-701B-4A32-9512-660098BBDF57}"/>
+    <hyperlink ref="D10" r:id="rId14" xr:uid="{A8923910-483F-46D2-8ED9-C10E6AF959E8}"/>
+    <hyperlink ref="D78" r:id="rId15" xr:uid="{DB2F31ED-A20B-4C8C-8687-199BB200EF6C}"/>
+    <hyperlink ref="D75" r:id="rId16" xr:uid="{7D001425-952B-4273-9E9A-FCE3CB5FFF9A}"/>
+    <hyperlink ref="D76" r:id="rId17" xr:uid="{156ECCF7-0BD4-43A9-B176-59C6D564886B}"/>
+    <hyperlink ref="D77" r:id="rId18" xr:uid="{918848D8-7BE5-4018-8C55-CEC7002CA9F2}"/>
+    <hyperlink ref="D79" r:id="rId19" xr:uid="{8E1E973E-3ACA-4E7C-AD67-B499DA21FEA1}"/>
+    <hyperlink ref="D80" r:id="rId20" xr:uid="{4FD46094-DAB9-4CD6-A190-C0C6227810FC}"/>
+    <hyperlink ref="D69" r:id="rId21" xr:uid="{7716567D-D933-48C2-9224-35CA8B300709}"/>
+    <hyperlink ref="D68" r:id="rId22" xr:uid="{6E2FCDC0-D3E2-4E28-9D42-F1F93D03797C}"/>
+    <hyperlink ref="D67" r:id="rId23" xr:uid="{417AACA0-6100-426E-85C1-0AF8CC02E529}"/>
+    <hyperlink ref="D66" r:id="rId24" xr:uid="{DAC37E6D-5373-4CEA-BF1C-8C46D88AC0DF}"/>
+    <hyperlink ref="D65" r:id="rId25" xr:uid="{1FD7B0EC-16E0-4C60-AE94-7B4720546328}"/>
+    <hyperlink ref="D30" r:id="rId26" xr:uid="{A75B96D2-F71B-42A6-87D0-363BA6BAFBD9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2833,19 +3664,19 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -2853,25 +3684,25 @@
         <v>54</v>
       </c>
       <c r="C1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" t="s">
         <v>133</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>134</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>135</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>137</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>138</v>
-      </c>
-      <c r="I1" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Column names standardized - Amazon
</commit_message>
<xml_diff>
--- a/data/Data Collection.xlsx
+++ b/data/Data Collection.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{8632A504-ECB9-41F3-83C2-D8FB0D9BADB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6ECBEC7-1754-4487-B5A7-BC71436C19A6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{EFA0F3B4-3249-4998-8A76-0DCAF9FCE7B8}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" firstSheet="1" activeTab="2" xr2:uid="{EFA0F3B4-3249-4998-8A76-0DCAF9FCE7B8}"/>
   </bookViews>
   <sheets>
     <sheet name="productCollectionList" sheetId="1" r:id="rId1"/>
@@ -1279,6 +1279,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2037,7 +2041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8FFCC8-FB4D-413C-81EB-800110419A65}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+    <sheetView zoomScale="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
@@ -3659,9 +3663,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F947BAD6-2752-4AC0-BEE3-804E058AF41F}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3707,5 +3711,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Amazon - All Products reviews
</commit_message>
<xml_diff>
--- a/data/Data Collection.xlsx
+++ b/data/Data Collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f943686c21a634a0/Desktop/Data Mining/CSCI-Final-Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{8632A504-ECB9-41F3-83C2-D8FB0D9BADB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6ECBEC7-1754-4487-B5A7-BC71436C19A6}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{8632A504-ECB9-41F3-83C2-D8FB0D9BADB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{046BAEDD-6383-4A0A-856D-8AC3943C8893}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" firstSheet="1" activeTab="2" xr2:uid="{EFA0F3B4-3249-4998-8A76-0DCAF9FCE7B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="1" xr2:uid="{EFA0F3B4-3249-4998-8A76-0DCAF9FCE7B8}"/>
   </bookViews>
   <sheets>
     <sheet name="productCollectionList" sheetId="1" r:id="rId1"/>
@@ -2041,9 +2041,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8FFCC8-FB4D-413C-81EB-800110419A65}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2825,7 +2825,7 @@
       <c r="C44" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="2" t="s">
         <v>239</v>
       </c>
       <c r="E44" s="1" t="s">
@@ -2860,7 +2860,7 @@
       <c r="C45" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="2" t="s">
         <v>243</v>
       </c>
       <c r="E45" s="1" t="s">
@@ -2895,7 +2895,7 @@
       <c r="C46" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="2" t="s">
         <v>247</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -3654,6 +3654,19 @@
     <hyperlink ref="D66" r:id="rId24" xr:uid="{DAC37E6D-5373-4CEA-BF1C-8C46D88AC0DF}"/>
     <hyperlink ref="D65" r:id="rId25" xr:uid="{1FD7B0EC-16E0-4C60-AE94-7B4720546328}"/>
     <hyperlink ref="D30" r:id="rId26" xr:uid="{A75B96D2-F71B-42A6-87D0-363BA6BAFBD9}"/>
+    <hyperlink ref="D35" r:id="rId27" xr:uid="{3D992E38-9A03-4F7D-AA92-E41A6651AC00}"/>
+    <hyperlink ref="D36" r:id="rId28" xr:uid="{834ED2DB-970C-48B6-9EFE-1A252515B6BB}"/>
+    <hyperlink ref="D37" r:id="rId29" xr:uid="{2C4D47A3-7193-44BA-A21E-EAED5940DF85}"/>
+    <hyperlink ref="D38" r:id="rId30" xr:uid="{DE78018A-E9A9-450A-BD0F-9A6470DBC4EC}"/>
+    <hyperlink ref="D39" r:id="rId31" xr:uid="{DED299E5-1F17-4BCE-A24B-3FC1E6C9521F}"/>
+    <hyperlink ref="D40" r:id="rId32" xr:uid="{8CAF0902-B308-4A95-86E8-8CBF4C16620A}"/>
+    <hyperlink ref="D41" r:id="rId33" xr:uid="{E4E1B484-946E-44B0-90BD-761798C9300B}"/>
+    <hyperlink ref="D42" r:id="rId34" xr:uid="{E87D0DF3-770B-4C30-8C47-5ABA6D448AAD}"/>
+    <hyperlink ref="D43" r:id="rId35" xr:uid="{C01CBC0F-8664-4EBD-A7B6-7AF4EFD4C0EB}"/>
+    <hyperlink ref="D44" r:id="rId36" xr:uid="{4D9B0924-88D7-4380-AB8C-8AD72CC3BFA3}"/>
+    <hyperlink ref="D45" r:id="rId37" xr:uid="{2BBC497B-150C-44DA-89F6-23DCA175AEBE}"/>
+    <hyperlink ref="D46" r:id="rId38" xr:uid="{3385D83A-585B-41CE-94AB-81E89CE78CD0}"/>
+    <hyperlink ref="D56" r:id="rId39" xr:uid="{FBBFB39F-8CF7-469F-A66B-E965EF7CAC20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3663,7 +3676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F947BAD6-2752-4AC0-BEE3-804E058AF41F}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>

</xml_diff>